<commit_message>
Added more ingredient info
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08C52CB-D138-4670-80E4-B9D8E3FC086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E712A3-D642-4E24-8369-5CE5B0D1B69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>Ingredient</t>
   </si>
@@ -93,9 +93,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>Cl</t>
-  </si>
-  <si>
     <t>Ca</t>
   </si>
   <si>
@@ -117,21 +114,9 @@
     <t>Mn</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>Sel</t>
   </si>
   <si>
-    <t>Cr</t>
-  </si>
-  <si>
-    <t>Mo</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>μg</t>
   </si>
   <si>
@@ -225,9 +210,6 @@
     <t>biotin</t>
   </si>
   <si>
-    <t>folic acid</t>
-  </si>
-  <si>
     <t>cobalamin</t>
   </si>
   <si>
@@ -241,6 +223,9 @@
   </si>
   <si>
     <t>phylloqu.</t>
+  </si>
+  <si>
+    <t>folate</t>
   </si>
 </sst>
 </file>
@@ -604,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,48 +605,48 @@
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>66</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -681,91 +666,76 @@
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -824,7 +794,7 @@
         <v>21</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>22</v>
@@ -851,27 +821,12 @@
         <v>29</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -889,9 +844,9 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>48</v>
@@ -926,6 +881,9 @@
       <c r="L5">
         <v>0.13800000000000001</v>
       </c>
+      <c r="N5">
+        <v>19</v>
+      </c>
       <c r="P5">
         <v>5.9</v>
       </c>
@@ -938,40 +896,37 @@
       <c r="T5">
         <v>320</v>
       </c>
+      <c r="U5">
+        <v>33</v>
+      </c>
       <c r="V5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="W5">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="X5">
-        <v>12</v>
+        <v>0.3</v>
       </c>
       <c r="Y5">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="Z5">
-        <v>0.24</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA5">
-        <v>4.4999999999999998E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="AB5">
-        <v>0.14299999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="AC5">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="AD5">
-        <v>0.1</v>
-      </c>
-      <c r="AH5">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>106</v>
@@ -989,9 +944,9 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>142</v>
@@ -1009,9 +964,9 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>322</v>
@@ -1028,10 +983,76 @@
       <c r="F8">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>381</v>
+      </c>
+      <c r="H8">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K8">
+        <v>2.99</v>
+      </c>
+      <c r="L8">
+        <v>0.35</v>
+      </c>
+      <c r="N8">
+        <v>146</v>
+      </c>
+      <c r="O8">
+        <v>1.95</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>5.4</v>
+      </c>
+      <c r="R8">
+        <v>2.58</v>
+      </c>
+      <c r="S8">
+        <v>0.7</v>
+      </c>
+      <c r="T8">
+        <v>109</v>
+      </c>
+      <c r="U8">
+        <v>129</v>
+      </c>
+      <c r="V8">
+        <v>390</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>2.73</v>
+      </c>
+      <c r="Y8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AA8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AB8">
+        <v>56</v>
+      </c>
+      <c r="AC8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>143</v>
@@ -1049,9 +1070,9 @@
         <v>6.62</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>357</v>
@@ -1069,9 +1090,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>340</v>
@@ -1088,10 +1109,70 @@
       <c r="F11">
         <v>2.84</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>411</v>
+      </c>
+      <c r="H11">
+        <v>0.02</v>
+      </c>
+      <c r="I11">
+        <v>0.188</v>
+      </c>
+      <c r="J11">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>0.16</v>
+      </c>
+      <c r="P11">
+        <v>0.6</v>
+      </c>
+      <c r="Q11">
+        <v>1.6</v>
+      </c>
+      <c r="R11">
+        <v>0.92</v>
+      </c>
+      <c r="S11">
+        <v>3.2</v>
+      </c>
+      <c r="T11">
+        <v>95</v>
+      </c>
+      <c r="U11">
+        <v>66</v>
+      </c>
+      <c r="V11">
+        <v>58</v>
+      </c>
+      <c r="W11">
+        <v>7</v>
+      </c>
+      <c r="X11">
+        <v>0.1</v>
+      </c>
+      <c r="Y11">
+        <v>0.24</v>
+      </c>
+      <c r="Z11">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>61</v>
@@ -1109,9 +1190,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>429</v>
@@ -1128,10 +1209,16 @@
       <c r="F13">
         <v>7.14</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>143</v>
+      </c>
+      <c r="AC13">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>61</v>
@@ -1148,10 +1235,58 @@
       <c r="F14">
         <v>3.27</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>32</v>
+      </c>
+      <c r="H14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.105</v>
+      </c>
+      <c r="L14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O14">
+        <v>0.54</v>
+      </c>
+      <c r="R14">
+        <v>0.05</v>
+      </c>
+      <c r="S14">
+        <v>0.3</v>
+      </c>
+      <c r="T14">
+        <v>150</v>
+      </c>
+      <c r="U14">
+        <v>123</v>
+      </c>
+      <c r="V14">
+        <v>101</v>
+      </c>
+      <c r="W14">
+        <v>12</v>
+      </c>
+      <c r="Y14">
+        <v>0.41</v>
+      </c>
+      <c r="Z14">
+        <v>1E-3</v>
+      </c>
+      <c r="AB14">
+        <v>1.9</v>
+      </c>
+      <c r="AC14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>884</v>
@@ -1177,19 +1312,19 @@
       <c r="T15">
         <v>1</v>
       </c>
-      <c r="V15">
+      <c r="U15">
         <v>1</v>
       </c>
-      <c r="Y15">
+      <c r="X15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AH15">
+      <c r="AC15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>36</v>
@@ -1207,9 +1342,9 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>371</v>
@@ -1235,13 +1370,13 @@
       <c r="J17">
         <v>5.36</v>
       </c>
-      <c r="Y17">
+      <c r="X17">
         <v>3.21</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>72</v>
@@ -1259,9 +1394,9 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -1296,6 +1431,9 @@
       <c r="L19">
         <v>6.0999999999999999E-2</v>
       </c>
+      <c r="N19">
+        <v>16</v>
+      </c>
       <c r="P19">
         <v>9</v>
       </c>
@@ -1308,37 +1446,37 @@
       <c r="T19">
         <v>340</v>
       </c>
+      <c r="U19">
+        <v>21</v>
+      </c>
       <c r="V19">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="W19">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="X19">
-        <v>12</v>
+        <v>0.8</v>
       </c>
       <c r="Y19">
-        <v>0.8</v>
+        <v>0.32</v>
       </c>
       <c r="Z19">
-        <v>0.32</v>
+        <v>0.127</v>
       </c>
       <c r="AA19">
-        <v>0.127</v>
+        <v>0.125</v>
       </c>
       <c r="AB19">
-        <v>0.125</v>
-      </c>
-      <c r="AD19">
         <v>0.3</v>
       </c>
-      <c r="AH19">
+      <c r="AC19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>359</v>
@@ -1355,10 +1493,61 @@
       <c r="F20">
         <v>6.94</v>
       </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I20">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J20">
+        <v>1.48</v>
+      </c>
+      <c r="K20">
+        <v>0.39</v>
+      </c>
+      <c r="L20">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N20">
+        <v>97</v>
+      </c>
+      <c r="R20">
+        <v>0.04</v>
+      </c>
+      <c r="T20">
+        <v>35</v>
+      </c>
+      <c r="U20">
+        <v>10</v>
+      </c>
+      <c r="V20">
+        <v>43</v>
+      </c>
+      <c r="W20">
+        <v>12</v>
+      </c>
+      <c r="X20">
+        <v>1.2</v>
+      </c>
+      <c r="Y20">
+        <v>0.49</v>
+      </c>
+      <c r="Z20">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA20">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB20">
+        <v>7.5</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>367</v>
@@ -1375,10 +1564,22 @@
       <c r="F21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>106</v>
+      </c>
+      <c r="U21">
+        <v>30</v>
+      </c>
+      <c r="X21">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AC21">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>385</v>
@@ -1395,10 +1596,34 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0.05</v>
+      </c>
+      <c r="Y22">
+        <v>0.01</v>
+      </c>
+      <c r="Z22">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB22">
+        <v>0.6</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -1433,6 +1658,9 @@
       <c r="L23">
         <v>0.08</v>
       </c>
+      <c r="N23">
+        <v>15</v>
+      </c>
       <c r="P23">
         <v>13.7</v>
       </c>
@@ -1445,28 +1673,25 @@
       <c r="T23">
         <v>237</v>
       </c>
+      <c r="U23">
+        <v>10</v>
+      </c>
       <c r="V23">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="W23">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="X23">
-        <v>11</v>
+        <v>0.27</v>
       </c>
       <c r="Y23">
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="Z23">
-        <v>0.17</v>
-      </c>
-      <c r="AA23">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC23">
-        <v>2.3E-3</v>
-      </c>
-      <c r="AH23">
         <v>5</v>
       </c>
     </row>
@@ -1688,7 +1913,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U1048576">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1700,7 +1925,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V1048576">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1712,7 +1937,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1724,7 +1949,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X1048576">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1736,7 +1961,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y1:Y1048576">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1748,7 +1973,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z1048576">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1760,7 +1985,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1772,7 +1997,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB1:AB1048576">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1784,66 +2009,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD1:AD1048576">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE1:AE1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG1:AG1048576">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH1:AH1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New recipes, changes to old ones
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B68D657-0281-4E08-9DFA-2E3FD994422F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4D98BD-AC94-463D-9C70-E609B1EB6659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20130" yWindow="1740" windowWidth="18135" windowHeight="16905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Ingredient</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>pork</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>cured cheese</t>
+  </si>
+  <si>
+    <t>pine nuts</t>
   </si>
 </sst>
 </file>
@@ -598,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,636 +844,705 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>0.64</v>
+      </c>
+      <c r="D4">
+        <v>2.65</v>
+      </c>
+      <c r="E4">
+        <v>0.3</v>
+      </c>
+      <c r="F4">
+        <v>3.15</v>
+      </c>
+      <c r="G4">
+        <v>264</v>
+      </c>
+      <c r="H4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="K4">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="L4">
+        <v>0.155</v>
+      </c>
+      <c r="N4">
         <v>68</v>
       </c>
-      <c r="B4">
-        <v>254</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>17.2</v>
-      </c>
-      <c r="G4">
+      <c r="P4">
+        <v>18</v>
+      </c>
+      <c r="R4">
+        <v>0.8</v>
+      </c>
+      <c r="S4">
+        <v>415</v>
+      </c>
+      <c r="T4">
+        <v>295</v>
+      </c>
+      <c r="U4">
+        <v>177</v>
+      </c>
+      <c r="V4">
+        <v>56</v>
+      </c>
+      <c r="W4">
+        <v>64</v>
+      </c>
+      <c r="X4">
+        <v>3.17</v>
+      </c>
+      <c r="Y4">
+        <v>0.81</v>
+      </c>
+      <c r="Z4">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AA4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AB4">
+        <v>0.3</v>
+      </c>
+      <c r="AC4">
         <v>4</v>
-      </c>
-      <c r="H4">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="I4">
-        <v>0.151</v>
-      </c>
-      <c r="J4">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="K4">
-        <v>0.498</v>
-      </c>
-      <c r="L4">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="N4">
-        <v>7</v>
-      </c>
-      <c r="O4">
-        <v>2.14</v>
-      </c>
-      <c r="Q4">
-        <v>0.1</v>
-      </c>
-      <c r="R4">
-        <v>0.17</v>
-      </c>
-      <c r="S4">
-        <v>1.8</v>
-      </c>
-      <c r="T4">
-        <v>270</v>
-      </c>
-      <c r="U4">
-        <v>18</v>
-      </c>
-      <c r="V4">
-        <v>158</v>
-      </c>
-      <c r="W4">
-        <v>17</v>
-      </c>
-      <c r="X4">
-        <v>1.94</v>
-      </c>
-      <c r="Y4">
-        <v>4.18</v>
-      </c>
-      <c r="Z4">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="AA4">
-        <v>0.01</v>
-      </c>
-      <c r="AB4">
-        <v>15</v>
-      </c>
-      <c r="AC4">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B5">
-        <v>32</v>
+        <v>254</v>
       </c>
       <c r="C5">
-        <v>0.16</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>6.7</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.88</v>
+        <v>17.2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.151</v>
+      </c>
+      <c r="J5">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="K5">
+        <v>0.498</v>
+      </c>
+      <c r="L5">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>2.14</v>
+      </c>
+      <c r="Q5">
+        <v>0.1</v>
+      </c>
+      <c r="R5">
+        <v>0.17</v>
+      </c>
+      <c r="S5">
+        <v>1.8</v>
+      </c>
+      <c r="T5">
+        <v>270</v>
+      </c>
+      <c r="U5">
+        <v>18</v>
+      </c>
+      <c r="V5">
+        <v>158</v>
+      </c>
+      <c r="W5">
+        <v>17</v>
+      </c>
+      <c r="X5">
+        <v>1.94</v>
+      </c>
+      <c r="Y5">
+        <v>4.18</v>
+      </c>
+      <c r="Z5">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AA5">
+        <v>0.01</v>
+      </c>
+      <c r="AB5">
+        <v>15</v>
+      </c>
+      <c r="AC5">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>0.35</v>
+        <v>0.16</v>
       </c>
       <c r="D6">
-        <v>10.3</v>
+        <v>6.7</v>
       </c>
       <c r="E6">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="F6">
-        <v>0.94</v>
-      </c>
-      <c r="G6">
-        <v>835</v>
-      </c>
-      <c r="H6">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I6">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J6">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="K6">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="L6">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="N6">
-        <v>19</v>
-      </c>
-      <c r="P6">
-        <v>5.9</v>
-      </c>
-      <c r="R6">
-        <v>0.66</v>
-      </c>
-      <c r="S6">
-        <v>13.2</v>
-      </c>
-      <c r="T6">
-        <v>320</v>
-      </c>
-      <c r="U6">
-        <v>33</v>
-      </c>
-      <c r="V6">
-        <v>35</v>
-      </c>
-      <c r="W6">
-        <v>12</v>
-      </c>
-      <c r="X6">
-        <v>0.3</v>
-      </c>
-      <c r="Y6">
-        <v>0.24</v>
-      </c>
-      <c r="Z6">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA6">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="AB6">
-        <v>0.1</v>
-      </c>
-      <c r="AC6">
-        <v>69</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C7">
-        <v>0.17</v>
+        <v>0.35</v>
       </c>
       <c r="D7">
-        <v>2.97</v>
+        <v>10.3</v>
       </c>
       <c r="E7">
-        <v>1.34</v>
+        <v>4.7</v>
       </c>
       <c r="F7">
-        <v>0.69</v>
+        <v>0.94</v>
       </c>
       <c r="G7">
-        <v>22</v>
+        <v>835</v>
       </c>
       <c r="H7">
-        <v>2.1000000000000001E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="I7">
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J7">
-        <v>0.32</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="K7">
-        <v>0.246</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="L7">
-        <v>7.3999999999999996E-2</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="N7">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="P7">
-        <v>3.1</v>
+        <v>5.9</v>
       </c>
       <c r="R7">
-        <v>0.27</v>
+        <v>0.66</v>
       </c>
       <c r="S7">
-        <v>29.3</v>
+        <v>13.2</v>
       </c>
       <c r="T7">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="U7">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="V7">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="W7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="Y7">
-        <v>0.13</v>
+        <v>0.24</v>
       </c>
       <c r="Z7">
-        <v>3.5000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA7">
-        <v>0.10299999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="AB7">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="AC7">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B8">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>1.93</v>
+        <v>0.17</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.97</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="F8">
-        <v>22.5</v>
+        <v>0.69</v>
+      </c>
+      <c r="G8">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.32</v>
+      </c>
+      <c r="K8">
+        <v>0.246</v>
+      </c>
+      <c r="L8">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N8">
+        <v>36</v>
+      </c>
+      <c r="P8">
+        <v>3.1</v>
+      </c>
+      <c r="R8">
+        <v>0.27</v>
+      </c>
+      <c r="S8">
+        <v>29.3</v>
+      </c>
+      <c r="T8">
+        <v>260</v>
+      </c>
+      <c r="U8">
+        <v>40</v>
+      </c>
+      <c r="V8">
+        <v>24</v>
+      </c>
+      <c r="W8">
+        <v>11</v>
+      </c>
+      <c r="X8">
+        <v>0.2</v>
+      </c>
+      <c r="Y8">
+        <v>0.13</v>
+      </c>
+      <c r="Z8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AB8">
+        <v>0.4</v>
+      </c>
+      <c r="AC8">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="C9">
-        <v>9.9600000000000009</v>
+        <v>1.93</v>
       </c>
       <c r="D9">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>12.4</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B10">
-        <v>322</v>
+        <v>420</v>
       </c>
       <c r="C10">
-        <v>26.5</v>
+        <v>27.8</v>
       </c>
       <c r="D10">
-        <v>3.59</v>
+        <v>13.9</v>
       </c>
       <c r="E10">
-        <v>0.56000000000000005</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F10">
-        <v>15.9</v>
+        <v>28.4</v>
       </c>
       <c r="G10">
-        <v>381</v>
+        <v>262</v>
       </c>
       <c r="H10">
-        <v>0.17599999999999999</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I10">
-        <v>0.52800000000000002</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="J10">
-        <v>2.4E-2</v>
+        <v>0.08</v>
       </c>
       <c r="K10">
-        <v>2.99</v>
+        <v>0.45</v>
       </c>
       <c r="L10">
-        <v>0.35</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="N10">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="O10">
-        <v>1.95</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="Q10">
-        <v>5.4</v>
+        <v>0.5</v>
       </c>
       <c r="R10">
-        <v>2.58</v>
+        <v>0.53</v>
       </c>
       <c r="S10">
-        <v>0.7</v>
+        <v>1.7</v>
       </c>
       <c r="T10">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="U10">
-        <v>129</v>
+        <v>853</v>
       </c>
       <c r="V10">
-        <v>390</v>
+        <v>627</v>
       </c>
       <c r="W10">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="X10">
-        <v>2.73</v>
+        <v>0.49</v>
       </c>
       <c r="Y10">
-        <v>2.2999999999999998</v>
+        <v>4.2</v>
       </c>
       <c r="Z10">
-        <v>7.6999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AA10">
-        <v>5.5E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="AB10">
-        <v>56</v>
+        <v>34.4</v>
       </c>
       <c r="AC10">
-        <v>48</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11">
-        <v>0.38</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D11">
-        <v>28.2</v>
+        <v>0.96</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F11">
-        <v>6.62</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="C12">
+        <v>26.5</v>
+      </c>
+      <c r="D12">
+        <v>3.59</v>
+      </c>
+      <c r="E12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F12">
+        <v>15.9</v>
+      </c>
+      <c r="G12">
+        <v>381</v>
+      </c>
+      <c r="H12">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J12">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K12">
+        <v>2.99</v>
+      </c>
+      <c r="L12">
+        <v>0.35</v>
+      </c>
+      <c r="N12">
+        <v>146</v>
+      </c>
+      <c r="O12">
+        <v>1.95</v>
+      </c>
+      <c r="P12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>89</v>
+      <c r="Q12">
+        <v>5.4</v>
+      </c>
+      <c r="R12">
+        <v>2.58</v>
+      </c>
+      <c r="S12">
+        <v>0.7</v>
+      </c>
+      <c r="T12">
+        <v>109</v>
+      </c>
+      <c r="U12">
+        <v>129</v>
+      </c>
+      <c r="V12">
+        <v>390</v>
+      </c>
+      <c r="W12">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>2.73</v>
+      </c>
+      <c r="Y12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z12">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AA12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AB12">
+        <v>56</v>
+      </c>
+      <c r="AC12">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13">
-        <v>340</v>
+        <v>143</v>
       </c>
       <c r="C13">
-        <v>36.1</v>
+        <v>0.38</v>
       </c>
       <c r="D13">
-        <v>2.9</v>
+        <v>28.2</v>
       </c>
       <c r="E13">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>2.84</v>
-      </c>
-      <c r="G13">
-        <v>411</v>
-      </c>
-      <c r="H13">
-        <v>0.02</v>
-      </c>
-      <c r="I13">
-        <v>0.188</v>
-      </c>
-      <c r="J13">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L13">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N13">
-        <v>4</v>
-      </c>
-      <c r="O13">
-        <v>0.16</v>
-      </c>
-      <c r="P13">
-        <v>0.6</v>
-      </c>
-      <c r="Q13">
-        <v>1.6</v>
-      </c>
-      <c r="R13">
-        <v>0.92</v>
-      </c>
-      <c r="S13">
-        <v>3.2</v>
-      </c>
-      <c r="T13">
-        <v>95</v>
-      </c>
-      <c r="U13">
-        <v>66</v>
-      </c>
-      <c r="V13">
-        <v>58</v>
-      </c>
-      <c r="W13">
-        <v>7</v>
-      </c>
-      <c r="X13">
-        <v>0.1</v>
-      </c>
-      <c r="Y13">
-        <v>0.24</v>
-      </c>
-      <c r="Z13">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB13">
-        <v>3</v>
-      </c>
-      <c r="AC13">
-        <v>27</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <v>61</v>
+        <v>357</v>
       </c>
       <c r="C14">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>1.5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15">
-        <v>429</v>
+        <v>340</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>36.1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="F15">
-        <v>7.14</v>
+        <v>2.84</v>
+      </c>
+      <c r="G15">
+        <v>411</v>
+      </c>
+      <c r="H15">
+        <v>0.02</v>
+      </c>
+      <c r="I15">
+        <v>0.188</v>
+      </c>
+      <c r="J15">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>0.16</v>
+      </c>
+      <c r="P15">
+        <v>0.6</v>
+      </c>
+      <c r="Q15">
+        <v>1.6</v>
+      </c>
+      <c r="R15">
+        <v>0.92</v>
+      </c>
+      <c r="S15">
+        <v>3.2</v>
+      </c>
+      <c r="T15">
+        <v>95</v>
       </c>
       <c r="U15">
-        <v>143</v>
+        <v>66</v>
+      </c>
+      <c r="V15">
+        <v>58</v>
+      </c>
+      <c r="W15">
+        <v>7</v>
+      </c>
+      <c r="X15">
+        <v>0.1</v>
+      </c>
+      <c r="Y15">
+        <v>0.24</v>
+      </c>
+      <c r="Z15">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB15">
+        <v>3</v>
       </c>
       <c r="AC15">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>61</v>
       </c>
       <c r="C16">
-        <v>3.2</v>
+        <v>0.3</v>
       </c>
       <c r="D16">
-        <v>4.9000000000000004</v>
+        <v>14</v>
       </c>
       <c r="E16">
-        <v>4.9000000000000004</v>
+        <v>3.9</v>
       </c>
       <c r="F16">
-        <v>3.27</v>
-      </c>
-      <c r="G16">
-        <v>32</v>
-      </c>
-      <c r="H16">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I16">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J16">
-        <v>0.105</v>
-      </c>
-      <c r="L16">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="O16">
-        <v>0.54</v>
-      </c>
-      <c r="R16">
-        <v>0.05</v>
-      </c>
-      <c r="S16">
-        <v>0.3</v>
-      </c>
-      <c r="T16">
-        <v>150</v>
-      </c>
-      <c r="U16">
-        <v>123</v>
-      </c>
-      <c r="V16">
-        <v>101</v>
-      </c>
-      <c r="W16">
-        <v>12</v>
-      </c>
-      <c r="Y16">
-        <v>0.41</v>
-      </c>
-      <c r="Z16">
-        <v>1E-3</v>
-      </c>
-      <c r="AB16">
-        <v>1.9</v>
-      </c>
-      <c r="AC16">
-        <v>38</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17">
-        <v>884</v>
+        <v>429</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1473,398 +1551,425 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>14.4</v>
-      </c>
-      <c r="S17">
-        <v>60.2</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
+        <v>7.14</v>
       </c>
       <c r="U17">
-        <v>1</v>
-      </c>
-      <c r="X17">
-        <v>0.56000000000000005</v>
+        <v>143</v>
       </c>
       <c r="AC17">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C18">
-        <v>0.13</v>
+        <v>3.2</v>
       </c>
       <c r="D18">
-        <v>7.68</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E18">
-        <v>5.76</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F18">
-        <v>0.89</v>
+        <v>3.27</v>
+      </c>
+      <c r="G18">
+        <v>32</v>
+      </c>
+      <c r="H18">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I18">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.105</v>
+      </c>
+      <c r="L18">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O18">
+        <v>0.54</v>
+      </c>
+      <c r="R18">
+        <v>0.05</v>
+      </c>
+      <c r="S18">
+        <v>0.3</v>
+      </c>
+      <c r="T18">
+        <v>150</v>
+      </c>
+      <c r="U18">
+        <v>123</v>
+      </c>
+      <c r="V18">
+        <v>101</v>
+      </c>
+      <c r="W18">
+        <v>12</v>
+      </c>
+      <c r="Y18">
+        <v>0.41</v>
+      </c>
+      <c r="Z18">
+        <v>1E-3</v>
+      </c>
+      <c r="AB18">
+        <v>1.9</v>
+      </c>
+      <c r="AC18">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19">
-        <v>371</v>
+        <v>884</v>
       </c>
       <c r="C19">
-        <v>1.51</v>
+        <v>100</v>
       </c>
       <c r="D19">
-        <v>74.67</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>13.04</v>
-      </c>
-      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>14.4</v>
+      </c>
+      <c r="S19">
+        <v>60.2</v>
+      </c>
+      <c r="T19">
         <v>1</v>
       </c>
-      <c r="I19">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J19">
-        <v>5.36</v>
+      <c r="U19">
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>3.21</v>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC19">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B20">
-        <v>263</v>
+        <v>36</v>
       </c>
       <c r="C20">
-        <v>21.2</v>
+        <v>0.13</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>7.68</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>5.76</v>
       </c>
       <c r="F20">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="I20">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="J20">
-        <v>4.34</v>
-      </c>
-      <c r="K20">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L20">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N20">
-        <v>5</v>
-      </c>
-      <c r="O20">
-        <v>0.7</v>
-      </c>
-      <c r="P20">
-        <v>0.7</v>
-      </c>
-      <c r="T20">
-        <v>287</v>
-      </c>
-      <c r="U20">
-        <v>14</v>
-      </c>
-      <c r="V20">
-        <v>175</v>
-      </c>
-      <c r="W20">
-        <v>19</v>
-      </c>
-      <c r="X20">
-        <v>0.88</v>
-      </c>
-      <c r="Y20">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z20">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA20">
-        <v>0.01</v>
-      </c>
-      <c r="AB20">
-        <v>24.6</v>
-      </c>
-      <c r="AC20">
-        <v>56</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21">
-        <v>72</v>
+        <v>371</v>
       </c>
       <c r="C21">
-        <v>0.26</v>
+        <v>1.51</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>74.67</v>
       </c>
       <c r="E21">
-        <v>0.65</v>
+        <v>2.7</v>
       </c>
       <c r="F21">
-        <v>1.81</v>
+        <v>13.04</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="J21">
+        <v>5.36</v>
+      </c>
+      <c r="X21">
+        <v>3.21</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B22">
-        <v>26</v>
+        <v>673</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>13.1</v>
       </c>
       <c r="E22">
-        <v>2.8</v>
+        <v>3.59</v>
       </c>
       <c r="F22">
+        <v>13.7</v>
+      </c>
+      <c r="G22">
         <v>1</v>
       </c>
-      <c r="G22">
-        <v>426</v>
-      </c>
       <c r="H22">
-        <v>0.05</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="I22">
-        <v>0.11</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="J22">
-        <v>0.6</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="K22">
-        <v>0.29799999999999999</v>
+        <v>0.313</v>
       </c>
       <c r="L22">
-        <v>6.0999999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="N22">
+        <v>34</v>
+      </c>
+      <c r="P22">
+        <v>0.8</v>
+      </c>
+      <c r="R22">
+        <v>9.33</v>
+      </c>
+      <c r="S22">
+        <v>53.9</v>
+      </c>
+      <c r="T22">
+        <v>597</v>
+      </c>
+      <c r="U22">
         <v>16</v>
       </c>
-      <c r="P22">
-        <v>9</v>
-      </c>
-      <c r="R22">
-        <v>1.06</v>
-      </c>
-      <c r="S22">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T22">
-        <v>340</v>
-      </c>
-      <c r="U22">
-        <v>21</v>
-      </c>
       <c r="V22">
-        <v>44</v>
+        <v>575</v>
       </c>
       <c r="W22">
-        <v>12</v>
+        <v>251</v>
       </c>
       <c r="X22">
-        <v>0.8</v>
+        <v>5.53</v>
       </c>
       <c r="Y22">
-        <v>0.32</v>
+        <v>6.45</v>
       </c>
       <c r="Z22">
-        <v>0.127</v>
+        <v>1.32</v>
       </c>
       <c r="AA22">
-        <v>0.125</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AB22">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AC22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B23">
-        <v>359</v>
+        <v>263</v>
       </c>
       <c r="C23">
-        <v>1.3</v>
+        <v>21.2</v>
       </c>
       <c r="D23">
-        <v>79.8</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>6.94</v>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>0.16300000000000001</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="I23">
-        <v>1.2999999999999999E-2</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="J23">
-        <v>1.48</v>
+        <v>4.34</v>
       </c>
       <c r="K23">
-        <v>0.39</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="L23">
-        <v>9.2999999999999999E-2</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="N23">
-        <v>97</v>
-      </c>
-      <c r="R23">
-        <v>0.04</v>
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>0.7</v>
+      </c>
+      <c r="P23">
+        <v>0.7</v>
       </c>
       <c r="T23">
-        <v>35</v>
+        <v>287</v>
       </c>
       <c r="U23">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="V23">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="W23">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X23">
-        <v>1.2</v>
+        <v>0.88</v>
       </c>
       <c r="Y23">
-        <v>0.49</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z23">
-        <v>6.9000000000000006E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA23">
-        <v>0.47199999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="AB23">
-        <v>7.5</v>
+        <v>24.6</v>
       </c>
       <c r="AC23">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24">
-        <v>367</v>
+        <v>72</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0.26</v>
       </c>
       <c r="D24">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="E24">
-        <v>40</v>
+        <v>0.65</v>
       </c>
       <c r="F24">
-        <v>7</v>
-      </c>
-      <c r="T24">
-        <v>106</v>
-      </c>
-      <c r="U24">
-        <v>30</v>
-      </c>
-      <c r="X24">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="AC24">
-        <v>106</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B25">
-        <v>385</v>
+        <v>26</v>
       </c>
       <c r="C25">
+        <v>0.1</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>2.8</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>426</v>
+      </c>
+      <c r="H25">
+        <v>0.05</v>
+      </c>
+      <c r="I25">
+        <v>0.11</v>
+      </c>
+      <c r="J25">
+        <v>0.6</v>
+      </c>
+      <c r="K25">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="L25">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N25">
+        <v>16</v>
+      </c>
+      <c r="P25">
+        <v>9</v>
+      </c>
+      <c r="R25">
+        <v>1.06</v>
+      </c>
+      <c r="S25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T25">
+        <v>340</v>
+      </c>
+      <c r="U25">
+        <v>21</v>
+      </c>
+      <c r="V25">
+        <v>44</v>
+      </c>
+      <c r="W25">
+        <v>12</v>
+      </c>
+      <c r="X25">
+        <v>0.8</v>
+      </c>
+      <c r="Y25">
         <v>0.32</v>
       </c>
-      <c r="D25">
-        <v>99.7</v>
-      </c>
-      <c r="E25">
-        <v>99.7</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>1.9E-2</v>
-      </c>
-      <c r="T25">
-        <v>2</v>
-      </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-      <c r="X25">
-        <v>0.05</v>
-      </c>
-      <c r="Y25">
-        <v>0.01</v>
-      </c>
       <c r="Z25">
-        <v>7.0000000000000001E-3</v>
+        <v>0.127</v>
+      </c>
+      <c r="AA25">
+        <v>0.125</v>
       </c>
       <c r="AB25">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="AC25">
         <v>1</v>
@@ -1872,75 +1977,222 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B26">
-        <v>18</v>
+        <v>359</v>
       </c>
       <c r="C26">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="D26">
-        <v>3.9</v>
+        <v>79.8</v>
       </c>
       <c r="E26">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.9</v>
-      </c>
-      <c r="G26">
-        <v>42</v>
+        <v>6.94</v>
       </c>
       <c r="H26">
-        <v>3.6999999999999998E-2</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="I26">
-        <v>1.9E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="J26">
-        <v>0.59399999999999997</v>
+        <v>1.48</v>
       </c>
       <c r="K26">
-        <v>8.8999999999999996E-2</v>
+        <v>0.39</v>
       </c>
       <c r="L26">
-        <v>0.08</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="N26">
-        <v>15</v>
-      </c>
-      <c r="P26">
-        <v>13.7</v>
+        <v>97</v>
       </c>
       <c r="R26">
-        <v>0.54</v>
-      </c>
-      <c r="S26">
-        <v>7.9</v>
+        <v>0.04</v>
       </c>
       <c r="T26">
-        <v>237</v>
+        <v>35</v>
       </c>
       <c r="U26">
         <v>10</v>
       </c>
       <c r="V26">
+        <v>43</v>
+      </c>
+      <c r="W26">
+        <v>12</v>
+      </c>
+      <c r="X26">
+        <v>1.2</v>
+      </c>
+      <c r="Y26">
+        <v>0.49</v>
+      </c>
+      <c r="Z26">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA26">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB26">
+        <v>7.5</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27">
+        <v>367</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>77</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="T27">
+        <v>106</v>
+      </c>
+      <c r="U27">
+        <v>30</v>
+      </c>
+      <c r="X27">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AC27">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>385</v>
+      </c>
+      <c r="C28">
+        <v>0.32</v>
+      </c>
+      <c r="D28">
+        <v>99.7</v>
+      </c>
+      <c r="E28">
+        <v>99.7</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T28">
+        <v>2</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>0.05</v>
+      </c>
+      <c r="Y28">
+        <v>0.01</v>
+      </c>
+      <c r="Z28">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB28">
+        <v>0.6</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>3.9</v>
+      </c>
+      <c r="E29">
+        <v>2.6</v>
+      </c>
+      <c r="F29">
+        <v>0.9</v>
+      </c>
+      <c r="G29">
+        <v>42</v>
+      </c>
+      <c r="H29">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I29">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J29">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="K29">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="L29">
+        <v>0.08</v>
+      </c>
+      <c r="N29">
+        <v>15</v>
+      </c>
+      <c r="P29">
+        <v>13.7</v>
+      </c>
+      <c r="R29">
+        <v>0.54</v>
+      </c>
+      <c r="S29">
+        <v>7.9</v>
+      </c>
+      <c r="T29">
+        <v>237</v>
+      </c>
+      <c r="U29">
+        <v>10</v>
+      </c>
+      <c r="V29">
         <v>24</v>
       </c>
-      <c r="W26">
+      <c r="W29">
         <v>11</v>
       </c>
-      <c r="X26">
+      <c r="X29">
         <v>0.27</v>
       </c>
-      <c r="Y26">
+      <c r="Y29">
         <v>0.17</v>
       </c>
-      <c r="Z26">
+      <c r="Z29">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AC26">
+      <c r="AC29">
         <v>5</v>
       </c>
     </row>
@@ -1993,7 +2245,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27:G1048576 H26 G1:G25">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:G1048576 H29 G1:G28">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2005,7 +2269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27:H1048576 I26 H1:H25">
+  <conditionalFormatting sqref="H30:H1048576 I29 H1:H28">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2017,7 +2281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I1048576 J26 I1:I25">
+  <conditionalFormatting sqref="I30:I1048576 J29 I1:I28">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2029,7 +2293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J27:J1048576 J1:J25">
+  <conditionalFormatting sqref="J30:J1048576 J1:J28">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2259,18 +2523,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="AC1:AC1048576">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
New utensil, new recipe
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CD796-9EB0-44EA-9F18-8406FDB1CC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C299348A-8B9F-41CD-8752-A018369BC42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>Ingredient</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>apple</t>
+  </si>
+  <si>
+    <t>guanciale</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,611 +1519,560 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B16">
-        <v>340</v>
+        <v>655</v>
       </c>
       <c r="C16">
-        <v>36.1</v>
+        <v>69.61</v>
       </c>
       <c r="D16">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>2.84</v>
-      </c>
-      <c r="G16">
-        <v>411</v>
-      </c>
-      <c r="H16">
-        <v>0.02</v>
-      </c>
-      <c r="I16">
-        <v>0.188</v>
-      </c>
-      <c r="J16">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N16">
-        <v>4</v>
-      </c>
-      <c r="O16">
-        <v>0.16</v>
-      </c>
-      <c r="P16">
-        <v>0.6</v>
-      </c>
-      <c r="Q16">
-        <v>1.6</v>
-      </c>
-      <c r="R16">
-        <v>0.92</v>
-      </c>
-      <c r="S16">
-        <v>3.2</v>
-      </c>
-      <c r="T16">
-        <v>95</v>
-      </c>
-      <c r="U16">
-        <v>66</v>
-      </c>
-      <c r="V16">
-        <v>58</v>
-      </c>
-      <c r="W16">
-        <v>7</v>
-      </c>
-      <c r="X16">
-        <v>0.1</v>
-      </c>
-      <c r="Y16">
-        <v>0.24</v>
-      </c>
-      <c r="Z16">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB16">
-        <v>3</v>
-      </c>
-      <c r="AC16">
-        <v>27</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
-        <v>61</v>
+        <v>340</v>
       </c>
       <c r="C17">
-        <v>0.3</v>
+        <v>36.1</v>
       </c>
       <c r="D17">
-        <v>14</v>
+        <v>2.9</v>
       </c>
       <c r="E17">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="F17">
-        <v>1.5</v>
+        <v>2.84</v>
+      </c>
+      <c r="G17">
+        <v>411</v>
+      </c>
+      <c r="H17">
+        <v>0.02</v>
+      </c>
+      <c r="I17">
+        <v>0.188</v>
+      </c>
+      <c r="J17">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>0.16</v>
+      </c>
+      <c r="P17">
+        <v>0.6</v>
+      </c>
+      <c r="Q17">
+        <v>1.6</v>
+      </c>
+      <c r="R17">
+        <v>0.92</v>
+      </c>
+      <c r="S17">
+        <v>3.2</v>
+      </c>
+      <c r="T17">
+        <v>95</v>
+      </c>
+      <c r="U17">
+        <v>66</v>
+      </c>
+      <c r="V17">
+        <v>58</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
+      <c r="X17">
+        <v>0.1</v>
+      </c>
+      <c r="Y17">
+        <v>0.24</v>
+      </c>
+      <c r="Z17">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB17">
+        <v>3</v>
+      </c>
+      <c r="AC17">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18">
-        <v>429</v>
+        <v>61</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>0.3</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="F18">
-        <v>7.14</v>
-      </c>
-      <c r="U18">
-        <v>143</v>
-      </c>
-      <c r="AC18">
-        <v>36</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19">
-        <v>61</v>
+        <v>429</v>
       </c>
       <c r="C19">
-        <v>3.2</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>4.9000000000000004</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>3.27</v>
-      </c>
-      <c r="G19">
-        <v>32</v>
-      </c>
-      <c r="H19">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I19">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J19">
-        <v>0.105</v>
-      </c>
-      <c r="L19">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="O19">
-        <v>0.54</v>
-      </c>
-      <c r="R19">
-        <v>0.05</v>
-      </c>
-      <c r="S19">
-        <v>0.3</v>
-      </c>
-      <c r="T19">
-        <v>150</v>
+        <v>7.14</v>
       </c>
       <c r="U19">
-        <v>123</v>
-      </c>
-      <c r="V19">
-        <v>101</v>
-      </c>
-      <c r="W19">
-        <v>12</v>
-      </c>
-      <c r="Y19">
-        <v>0.41</v>
-      </c>
-      <c r="Z19">
-        <v>1E-3</v>
-      </c>
-      <c r="AB19">
-        <v>1.9</v>
+        <v>143</v>
       </c>
       <c r="AC19">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
-        <v>884</v>
+        <v>61</v>
       </c>
       <c r="C20">
-        <v>100</v>
+        <v>3.2</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>3.27</v>
+      </c>
+      <c r="G20">
+        <v>32</v>
+      </c>
+      <c r="H20">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J20">
+        <v>0.105</v>
+      </c>
+      <c r="L20">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O20">
+        <v>0.54</v>
       </c>
       <c r="R20">
-        <v>14.4</v>
+        <v>0.05</v>
       </c>
       <c r="S20">
-        <v>60.2</v>
+        <v>0.3</v>
       </c>
       <c r="T20">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="U20">
-        <v>1</v>
-      </c>
-      <c r="X20">
-        <v>0.56000000000000005</v>
+        <v>123</v>
+      </c>
+      <c r="V20">
+        <v>101</v>
+      </c>
+      <c r="W20">
+        <v>12</v>
+      </c>
+      <c r="Y20">
+        <v>0.41</v>
+      </c>
+      <c r="Z20">
+        <v>1E-3</v>
+      </c>
+      <c r="AB20">
+        <v>1.9</v>
       </c>
       <c r="AC20">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21">
-        <v>36</v>
+        <v>884</v>
       </c>
       <c r="C21">
-        <v>0.13</v>
+        <v>100</v>
       </c>
       <c r="D21">
-        <v>7.68</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>5.76</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.89</v>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>14.4</v>
+      </c>
+      <c r="S21">
+        <v>60.2</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22">
-        <v>371</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <v>1.51</v>
+        <v>0.13</v>
       </c>
       <c r="D22">
-        <v>74.67</v>
+        <v>7.68</v>
       </c>
       <c r="E22">
-        <v>2.7</v>
+        <v>5.76</v>
       </c>
       <c r="F22">
-        <v>13.04</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J22">
-        <v>5.36</v>
-      </c>
-      <c r="X22">
-        <v>3.21</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B23">
-        <v>673</v>
+        <v>371</v>
       </c>
       <c r="C23">
-        <v>68.400000000000006</v>
+        <v>1.51</v>
       </c>
       <c r="D23">
-        <v>13.1</v>
+        <v>74.67</v>
       </c>
       <c r="E23">
-        <v>3.59</v>
+        <v>2.7</v>
       </c>
       <c r="F23">
-        <v>13.7</v>
-      </c>
-      <c r="G23">
+        <v>13.04</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
-      <c r="H23">
-        <v>0.36399999999999999</v>
-      </c>
       <c r="I23">
-        <v>0.22700000000000001</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J23">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="K23">
-        <v>0.313</v>
-      </c>
-      <c r="L23">
-        <v>9.4E-2</v>
-      </c>
-      <c r="N23">
-        <v>34</v>
-      </c>
-      <c r="P23">
-        <v>0.8</v>
-      </c>
-      <c r="R23">
-        <v>9.33</v>
-      </c>
-      <c r="S23">
-        <v>53.9</v>
-      </c>
-      <c r="T23">
-        <v>597</v>
-      </c>
-      <c r="U23">
-        <v>16</v>
-      </c>
-      <c r="V23">
-        <v>575</v>
-      </c>
-      <c r="W23">
-        <v>251</v>
+        <v>5.36</v>
       </c>
       <c r="X23">
-        <v>5.53</v>
-      </c>
-      <c r="Y23">
-        <v>6.45</v>
-      </c>
-      <c r="Z23">
-        <v>1.32</v>
-      </c>
-      <c r="AA23">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AB23">
-        <v>0.7</v>
-      </c>
-      <c r="AC23">
-        <v>2</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B24">
-        <v>263</v>
+        <v>673</v>
       </c>
       <c r="C24">
-        <v>21.2</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3.59</v>
       </c>
       <c r="F24">
-        <v>16.899999999999999</v>
+        <v>13.7</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J24">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K24">
+        <v>0.313</v>
+      </c>
+      <c r="L24">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N24">
+        <v>34</v>
+      </c>
+      <c r="P24">
+        <v>0.8</v>
+      </c>
+      <c r="R24">
+        <v>9.33</v>
+      </c>
+      <c r="S24">
+        <v>53.9</v>
+      </c>
+      <c r="T24">
+        <v>597</v>
+      </c>
+      <c r="U24">
+        <v>16</v>
+      </c>
+      <c r="V24">
+        <v>575</v>
+      </c>
+      <c r="W24">
+        <v>251</v>
+      </c>
+      <c r="X24">
+        <v>5.53</v>
+      </c>
+      <c r="Y24">
+        <v>6.45</v>
+      </c>
+      <c r="Z24">
+        <v>1.32</v>
+      </c>
+      <c r="AA24">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AB24">
+        <v>0.7</v>
+      </c>
+      <c r="AC24">
         <v>2</v>
-      </c>
-      <c r="H24">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="I24">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="J24">
-        <v>4.34</v>
-      </c>
-      <c r="K24">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L24">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
-      </c>
-      <c r="O24">
-        <v>0.7</v>
-      </c>
-      <c r="P24">
-        <v>0.7</v>
-      </c>
-      <c r="T24">
-        <v>287</v>
-      </c>
-      <c r="U24">
-        <v>14</v>
-      </c>
-      <c r="V24">
-        <v>175</v>
-      </c>
-      <c r="W24">
-        <v>19</v>
-      </c>
-      <c r="X24">
-        <v>0.88</v>
-      </c>
-      <c r="Y24">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z24">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA24">
-        <v>0.01</v>
-      </c>
-      <c r="AB24">
-        <v>24.6</v>
-      </c>
-      <c r="AC24">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B25">
-        <v>72</v>
+        <v>263</v>
       </c>
       <c r="C25">
-        <v>0.26</v>
+        <v>21.2</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1.81</v>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="I25">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="J25">
+        <v>4.34</v>
+      </c>
+      <c r="K25">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="L25">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="N25">
+        <v>5</v>
+      </c>
+      <c r="O25">
+        <v>0.7</v>
+      </c>
+      <c r="P25">
+        <v>0.7</v>
+      </c>
+      <c r="T25">
+        <v>287</v>
+      </c>
+      <c r="U25">
+        <v>14</v>
+      </c>
+      <c r="V25">
+        <v>175</v>
+      </c>
+      <c r="W25">
+        <v>19</v>
+      </c>
+      <c r="X25">
+        <v>0.88</v>
+      </c>
+      <c r="Y25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AA25">
+        <v>0.01</v>
+      </c>
+      <c r="AB25">
+        <v>24.6</v>
+      </c>
+      <c r="AC25">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E26">
-        <v>2.8</v>
+        <v>0.65</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>426</v>
-      </c>
-      <c r="H26">
-        <v>0.05</v>
-      </c>
-      <c r="I26">
-        <v>0.11</v>
-      </c>
-      <c r="J26">
-        <v>0.6</v>
-      </c>
-      <c r="K26">
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="L26">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="N26">
-        <v>16</v>
-      </c>
-      <c r="P26">
-        <v>9</v>
-      </c>
-      <c r="R26">
-        <v>1.06</v>
-      </c>
-      <c r="S26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T26">
-        <v>340</v>
-      </c>
-      <c r="U26">
-        <v>21</v>
-      </c>
-      <c r="V26">
-        <v>44</v>
-      </c>
-      <c r="W26">
-        <v>12</v>
-      </c>
-      <c r="X26">
-        <v>0.8</v>
-      </c>
-      <c r="Y26">
-        <v>0.32</v>
-      </c>
-      <c r="Z26">
-        <v>0.127</v>
-      </c>
-      <c r="AA26">
-        <v>0.125</v>
-      </c>
-      <c r="AB26">
-        <v>0.3</v>
-      </c>
-      <c r="AC26">
-        <v>1</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27">
-        <v>359</v>
+        <v>26</v>
       </c>
       <c r="C27">
-        <v>1.3</v>
+        <v>0.1</v>
       </c>
       <c r="D27">
-        <v>79.8</v>
+        <v>7</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="F27">
-        <v>6.94</v>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>426</v>
       </c>
       <c r="H27">
-        <v>0.16300000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="I27">
-        <v>1.2999999999999999E-2</v>
+        <v>0.11</v>
       </c>
       <c r="J27">
-        <v>1.48</v>
+        <v>0.6</v>
       </c>
       <c r="K27">
-        <v>0.39</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="L27">
-        <v>9.2999999999999999E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="N27">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="P27">
+        <v>9</v>
       </c>
       <c r="R27">
-        <v>0.04</v>
+        <v>1.06</v>
+      </c>
+      <c r="S27">
+        <v>1.1000000000000001</v>
       </c>
       <c r="T27">
-        <v>35</v>
+        <v>340</v>
       </c>
       <c r="U27">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="V27">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W27">
         <v>12</v>
       </c>
       <c r="X27">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="Y27">
-        <v>0.49</v>
+        <v>0.32</v>
       </c>
       <c r="Z27">
-        <v>6.9000000000000006E-2</v>
+        <v>0.127</v>
       </c>
       <c r="AA27">
-        <v>0.47199999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="AB27">
-        <v>7.5</v>
+        <v>0.3</v>
       </c>
       <c r="AC27">
         <v>1</v>
@@ -2128,151 +2080,222 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="D28">
-        <v>77</v>
+        <v>79.8</v>
       </c>
       <c r="E28">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>6.94</v>
+      </c>
+      <c r="H28">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J28">
+        <v>1.48</v>
+      </c>
+      <c r="K28">
+        <v>0.39</v>
+      </c>
+      <c r="L28">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N28">
+        <v>97</v>
+      </c>
+      <c r="R28">
+        <v>0.04</v>
       </c>
       <c r="T28">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="U28">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="V28">
+        <v>43</v>
+      </c>
+      <c r="W28">
+        <v>12</v>
       </c>
       <c r="X28">
-        <v>1.0900000000000001</v>
+        <v>1.2</v>
+      </c>
+      <c r="Y28">
+        <v>0.49</v>
+      </c>
+      <c r="Z28">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA28">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB28">
+        <v>7.5</v>
       </c>
       <c r="AC28">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="C29">
-        <v>0.32</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>99.7</v>
+        <v>77</v>
       </c>
       <c r="E29">
-        <v>99.7</v>
+        <v>40</v>
       </c>
       <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>1.9E-2</v>
+        <v>7</v>
       </c>
       <c r="T29">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="U29">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="X29">
-        <v>0.05</v>
-      </c>
-      <c r="Y29">
-        <v>0.01</v>
-      </c>
-      <c r="Z29">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB29">
-        <v>0.6</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="AC29">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>385</v>
       </c>
       <c r="C30">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="D30">
-        <v>3.9</v>
+        <v>99.7</v>
       </c>
       <c r="E30">
-        <v>2.6</v>
+        <v>99.7</v>
       </c>
       <c r="F30">
-        <v>0.9</v>
-      </c>
-      <c r="G30">
-        <v>42</v>
-      </c>
-      <c r="H30">
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>1.9E-2</v>
       </c>
-      <c r="J30">
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>0.05</v>
+      </c>
+      <c r="Y30">
+        <v>0.01</v>
+      </c>
+      <c r="Z30">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB30">
+        <v>0.6</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>0.2</v>
+      </c>
+      <c r="D31">
+        <v>3.9</v>
+      </c>
+      <c r="E31">
+        <v>2.6</v>
+      </c>
+      <c r="F31">
+        <v>0.9</v>
+      </c>
+      <c r="G31">
+        <v>42</v>
+      </c>
+      <c r="H31">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I31">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J31">
         <v>0.59399999999999997</v>
       </c>
-      <c r="K30">
+      <c r="K31">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="L30">
+      <c r="L31">
         <v>0.08</v>
       </c>
-      <c r="N30">
+      <c r="N31">
         <v>15</v>
       </c>
-      <c r="P30">
+      <c r="P31">
         <v>13.7</v>
       </c>
-      <c r="R30">
+      <c r="R31">
         <v>0.54</v>
       </c>
-      <c r="S30">
+      <c r="S31">
         <v>7.9</v>
       </c>
-      <c r="T30">
+      <c r="T31">
         <v>237</v>
       </c>
-      <c r="U30">
+      <c r="U31">
         <v>10</v>
       </c>
-      <c r="V30">
+      <c r="V31">
         <v>24</v>
       </c>
-      <c r="W30">
+      <c r="W31">
         <v>11</v>
       </c>
-      <c r="X30">
+      <c r="X31">
         <v>0.27</v>
       </c>
-      <c r="Y30">
+      <c r="Y31">
         <v>0.17</v>
       </c>
-      <c r="Z30">
+      <c r="Z31">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AC30">
+      <c r="AC31">
         <v>5</v>
       </c>
     </row>
@@ -2337,7 +2360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31:G1048576 H30 G1:G29">
+  <conditionalFormatting sqref="G32:G1048576 H31 G1:G30">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2349,7 +2372,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31:H1048576 I30 H1:H29">
+  <conditionalFormatting sqref="H32:H1048576 I31 H1:H30">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2361,7 +2384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I1048576 J30 I1:I29">
+  <conditionalFormatting sqref="I32:I1048576 J31 I1:I30">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2373,7 +2396,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J1048576 J1:J29">
+  <conditionalFormatting sqref="J32:J1048576 J1:J30">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New recipes, new table field...
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C299348A-8B9F-41CD-8752-A018369BC42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159C2AE-26BB-4981-BFAD-8CDEFF9872DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>Ingredient</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>guanciale</t>
+  </si>
+  <si>
+    <t>strawberries</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC31"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,119 +2186,172 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B30">
-        <v>385</v>
+        <v>36</v>
       </c>
       <c r="C30">
-        <v>0.32</v>
+        <v>0.22</v>
       </c>
       <c r="D30">
-        <v>99.7</v>
+        <v>7.96</v>
       </c>
       <c r="E30">
-        <v>99.7</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>1.9E-2</v>
+        <v>0.64</v>
+      </c>
+      <c r="M30">
+        <v>3.7</v>
+      </c>
+      <c r="P30">
+        <v>59.6</v>
       </c>
       <c r="T30">
+        <v>161</v>
+      </c>
+      <c r="U30">
+        <v>17</v>
+      </c>
+      <c r="V30">
+        <v>23</v>
+      </c>
+      <c r="W30">
+        <v>12.5</v>
+      </c>
+      <c r="X30">
+        <v>0.26</v>
+      </c>
+      <c r="Y30">
+        <v>0.11</v>
+      </c>
+      <c r="Z30">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA30">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AC30">
         <v>2</v>
-      </c>
-      <c r="U30">
-        <v>1</v>
-      </c>
-      <c r="X30">
-        <v>0.05</v>
-      </c>
-      <c r="Y30">
-        <v>0.01</v>
-      </c>
-      <c r="Z30">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB30">
-        <v>0.6</v>
-      </c>
-      <c r="AC30">
-        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>385</v>
       </c>
       <c r="C31">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="D31">
-        <v>3.9</v>
+        <v>99.7</v>
       </c>
       <c r="E31">
-        <v>2.6</v>
+        <v>99.7</v>
       </c>
       <c r="F31">
-        <v>0.9</v>
-      </c>
-      <c r="G31">
-        <v>42</v>
-      </c>
-      <c r="H31">
-        <v>3.6999999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>1.9E-2</v>
       </c>
-      <c r="J31">
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>0.05</v>
+      </c>
+      <c r="Y31">
+        <v>0.01</v>
+      </c>
+      <c r="Z31">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB31">
+        <v>0.6</v>
+      </c>
+      <c r="AC31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32">
+        <v>18</v>
+      </c>
+      <c r="C32">
+        <v>0.2</v>
+      </c>
+      <c r="D32">
+        <v>3.9</v>
+      </c>
+      <c r="E32">
+        <v>2.6</v>
+      </c>
+      <c r="F32">
+        <v>0.9</v>
+      </c>
+      <c r="G32">
+        <v>42</v>
+      </c>
+      <c r="H32">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I32">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J32">
         <v>0.59399999999999997</v>
       </c>
-      <c r="K31">
+      <c r="K32">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="L31">
+      <c r="L32">
         <v>0.08</v>
       </c>
-      <c r="N31">
+      <c r="N32">
         <v>15</v>
       </c>
-      <c r="P31">
+      <c r="P32">
         <v>13.7</v>
       </c>
-      <c r="R31">
+      <c r="R32">
         <v>0.54</v>
       </c>
-      <c r="S31">
+      <c r="S32">
         <v>7.9</v>
       </c>
-      <c r="T31">
+      <c r="T32">
         <v>237</v>
       </c>
-      <c r="U31">
+      <c r="U32">
         <v>10</v>
       </c>
-      <c r="V31">
+      <c r="V32">
         <v>24</v>
       </c>
-      <c r="W31">
+      <c r="W32">
         <v>11</v>
       </c>
-      <c r="X31">
+      <c r="X32">
         <v>0.27</v>
       </c>
-      <c r="Y31">
+      <c r="Y32">
         <v>0.17</v>
       </c>
-      <c r="Z31">
+      <c r="Z32">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AC31">
+      <c r="AC32">
         <v>5</v>
       </c>
     </row>
@@ -2360,7 +2416,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G1048576 H31 G1:G30">
+  <conditionalFormatting sqref="G33:G1048576 H32 G1:G31">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2372,7 +2428,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H1048576 I31 H1:H30">
+  <conditionalFormatting sqref="H33:H1048576 I32 H1:H31">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2384,7 +2440,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I1048576 J31 I1:I30">
+  <conditionalFormatting sqref="I33:I1048576 J32 I1:I31">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2396,7 +2452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32:J1048576 J1:J30">
+  <conditionalFormatting sqref="J33:J1048576 J1:J31">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
3 new recipes, corrections, new utensils, changed difficulty icon color...
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159C2AE-26BB-4981-BFAD-8CDEFF9872DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E555EDCF-04B4-42B7-A588-7918C6A51B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>Ingredient</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>strawberries</t>
+  </si>
+  <si>
+    <t>gofio</t>
+  </si>
+  <si>
+    <t>chickpeas</t>
+  </si>
+  <si>
+    <t>green beans</t>
+  </si>
+  <si>
+    <t>cabbage</t>
+  </si>
+  <si>
+    <t>cob of corn</t>
   </si>
 </sst>
 </file>
@@ -616,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB30" sqref="AB30"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,636 +1128,525 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="B8">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="D8">
-        <v>10.3</v>
+        <v>5.8</v>
       </c>
       <c r="E8">
-        <v>4.7</v>
+        <v>3.2</v>
       </c>
       <c r="F8">
-        <v>0.94</v>
-      </c>
-      <c r="G8">
-        <v>835</v>
-      </c>
-      <c r="H8">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I8">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J8">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="K8">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="L8">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="N8">
-        <v>19</v>
-      </c>
-      <c r="P8">
-        <v>5.9</v>
-      </c>
-      <c r="R8">
-        <v>0.66</v>
-      </c>
-      <c r="S8">
-        <v>13.2</v>
-      </c>
-      <c r="T8">
-        <v>320</v>
-      </c>
-      <c r="U8">
-        <v>33</v>
-      </c>
-      <c r="V8">
-        <v>35</v>
-      </c>
-      <c r="W8">
-        <v>12</v>
-      </c>
-      <c r="X8">
-        <v>0.3</v>
-      </c>
-      <c r="Y8">
-        <v>0.24</v>
-      </c>
-      <c r="Z8">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA8">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="AB8">
-        <v>0.1</v>
-      </c>
-      <c r="AC8">
-        <v>69</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C9">
-        <v>0.17</v>
+        <v>0.35</v>
       </c>
       <c r="D9">
-        <v>2.97</v>
+        <v>10.3</v>
       </c>
       <c r="E9">
-        <v>1.34</v>
+        <v>4.7</v>
       </c>
       <c r="F9">
-        <v>0.69</v>
+        <v>0.94</v>
       </c>
       <c r="G9">
-        <v>22</v>
+        <v>835</v>
       </c>
       <c r="H9">
-        <v>2.1000000000000001E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="I9">
-        <v>5.7000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="J9">
-        <v>0.32</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="K9">
-        <v>0.246</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="L9">
-        <v>7.3999999999999996E-2</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="N9">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="P9">
-        <v>3.1</v>
+        <v>5.9</v>
       </c>
       <c r="R9">
-        <v>0.27</v>
+        <v>0.66</v>
       </c>
       <c r="S9">
-        <v>29.3</v>
+        <v>13.2</v>
       </c>
       <c r="T9">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="U9">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="V9">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="W9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X9">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="Y9">
-        <v>0.13</v>
+        <v>0.24</v>
       </c>
       <c r="Z9">
-        <v>3.5000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA9">
-        <v>0.10299999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="AB9">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="AC9">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B10">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>1.93</v>
+        <v>0.17</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2.97</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1.34</v>
       </c>
       <c r="F10">
-        <v>22.5</v>
+        <v>0.69</v>
+      </c>
+      <c r="G10">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.32</v>
+      </c>
+      <c r="K10">
+        <v>0.246</v>
+      </c>
+      <c r="L10">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N10">
+        <v>36</v>
+      </c>
+      <c r="P10">
+        <v>3.1</v>
+      </c>
+      <c r="R10">
+        <v>0.27</v>
+      </c>
+      <c r="S10">
+        <v>29.3</v>
+      </c>
+      <c r="T10">
+        <v>260</v>
+      </c>
+      <c r="U10">
+        <v>40</v>
+      </c>
+      <c r="V10">
+        <v>24</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="X10">
+        <v>0.2</v>
+      </c>
+      <c r="Y10">
+        <v>0.13</v>
+      </c>
+      <c r="Z10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA10">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AB10">
+        <v>0.4</v>
+      </c>
+      <c r="AC10">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B11">
-        <v>420</v>
+        <v>106</v>
       </c>
       <c r="C11">
-        <v>27.8</v>
+        <v>1.93</v>
       </c>
       <c r="D11">
-        <v>13.9</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>28.4</v>
-      </c>
-      <c r="G11">
-        <v>262</v>
-      </c>
-      <c r="H11">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I11">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="J11">
-        <v>0.08</v>
-      </c>
-      <c r="K11">
-        <v>0.45</v>
-      </c>
-      <c r="L11">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="N11">
-        <v>6</v>
-      </c>
-      <c r="O11">
-        <v>1.4</v>
-      </c>
-      <c r="Q11">
-        <v>0.5</v>
-      </c>
-      <c r="R11">
-        <v>0.53</v>
-      </c>
-      <c r="S11">
-        <v>1.7</v>
-      </c>
-      <c r="T11">
-        <v>180</v>
-      </c>
-      <c r="U11">
-        <v>853</v>
-      </c>
-      <c r="V11">
-        <v>627</v>
-      </c>
-      <c r="W11">
-        <v>34</v>
-      </c>
-      <c r="X11">
-        <v>0.49</v>
-      </c>
-      <c r="Y11">
-        <v>4.2</v>
-      </c>
-      <c r="Z11">
-        <v>0.04</v>
-      </c>
-      <c r="AA11">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="AB11">
-        <v>34.4</v>
-      </c>
-      <c r="AC11">
-        <v>1800</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B12">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C12">
-        <v>9.9600000000000009</v>
+        <v>1.7</v>
       </c>
       <c r="D12">
-        <v>0.96</v>
+        <v>14.2</v>
       </c>
       <c r="E12">
         <v>0.2</v>
       </c>
       <c r="F12">
-        <v>12.4</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B13">
-        <v>322</v>
+        <v>86</v>
       </c>
       <c r="C13">
-        <v>26.5</v>
+        <v>1.35</v>
       </c>
       <c r="D13">
-        <v>3.59</v>
+        <v>18.7</v>
       </c>
       <c r="E13">
-        <v>0.56000000000000005</v>
+        <v>6.26</v>
       </c>
       <c r="F13">
-        <v>15.9</v>
-      </c>
-      <c r="G13">
-        <v>381</v>
-      </c>
-      <c r="H13">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="I13">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="J13">
-        <v>2.4E-2</v>
-      </c>
-      <c r="K13">
-        <v>2.99</v>
-      </c>
-      <c r="L13">
-        <v>0.35</v>
-      </c>
-      <c r="N13">
-        <v>146</v>
-      </c>
-      <c r="O13">
-        <v>1.95</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>5.4</v>
-      </c>
-      <c r="R13">
-        <v>2.58</v>
-      </c>
-      <c r="S13">
-        <v>0.7</v>
-      </c>
-      <c r="T13">
-        <v>109</v>
-      </c>
-      <c r="U13">
-        <v>129</v>
-      </c>
-      <c r="V13">
-        <v>390</v>
-      </c>
-      <c r="W13">
-        <v>5</v>
-      </c>
-      <c r="X13">
-        <v>2.73</v>
-      </c>
-      <c r="Y13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Z13">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="AA13">
-        <v>5.5E-2</v>
-      </c>
-      <c r="AB13">
-        <v>56</v>
-      </c>
-      <c r="AC13">
-        <v>48</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B14">
-        <v>143</v>
+        <v>420</v>
       </c>
       <c r="C14">
-        <v>0.38</v>
+        <v>27.8</v>
       </c>
       <c r="D14">
-        <v>28.2</v>
+        <v>13.9</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F14">
-        <v>6.62</v>
+        <v>28.4</v>
+      </c>
+      <c r="G14">
+        <v>262</v>
+      </c>
+      <c r="H14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J14">
+        <v>0.08</v>
+      </c>
+      <c r="K14">
+        <v>0.45</v>
+      </c>
+      <c r="L14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>1.4</v>
+      </c>
+      <c r="Q14">
+        <v>0.5</v>
+      </c>
+      <c r="R14">
+        <v>0.53</v>
+      </c>
+      <c r="S14">
+        <v>1.7</v>
+      </c>
+      <c r="T14">
+        <v>180</v>
+      </c>
+      <c r="U14">
+        <v>853</v>
+      </c>
+      <c r="V14">
+        <v>627</v>
+      </c>
+      <c r="W14">
+        <v>34</v>
+      </c>
+      <c r="X14">
+        <v>0.49</v>
+      </c>
+      <c r="Y14">
+        <v>4.2</v>
+      </c>
+      <c r="Z14">
+        <v>0.04</v>
+      </c>
+      <c r="AA14">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AB14">
+        <v>34.4</v>
+      </c>
+      <c r="AC14">
+        <v>1800</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15">
-        <v>357</v>
+        <v>142</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F15">
-        <v>89</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B16">
-        <v>655</v>
+        <v>322</v>
       </c>
       <c r="C16">
-        <v>69.61</v>
+        <v>26.5</v>
       </c>
       <c r="D16">
+        <v>3.59</v>
+      </c>
+      <c r="E16">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F16">
+        <v>15.9</v>
+      </c>
+      <c r="G16">
+        <v>381</v>
+      </c>
+      <c r="H16">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J16">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K16">
+        <v>2.99</v>
+      </c>
+      <c r="L16">
+        <v>0.35</v>
+      </c>
+      <c r="N16">
+        <v>146</v>
+      </c>
+      <c r="O16">
+        <v>1.95</v>
+      </c>
+      <c r="P16">
         <v>0</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>6.38</v>
+      <c r="Q16">
+        <v>5.4</v>
+      </c>
+      <c r="R16">
+        <v>2.58</v>
+      </c>
+      <c r="S16">
+        <v>0.7</v>
+      </c>
+      <c r="T16">
+        <v>109</v>
+      </c>
+      <c r="U16">
+        <v>129</v>
+      </c>
+      <c r="V16">
+        <v>390</v>
+      </c>
+      <c r="W16">
+        <v>5</v>
+      </c>
+      <c r="X16">
+        <v>2.73</v>
+      </c>
+      <c r="Y16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z16">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AA16">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AB16">
+        <v>56</v>
+      </c>
+      <c r="AC16">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17">
-        <v>340</v>
+        <v>143</v>
       </c>
       <c r="C17">
-        <v>36.1</v>
+        <v>0.38</v>
       </c>
       <c r="D17">
-        <v>2.9</v>
+        <v>28.2</v>
       </c>
       <c r="E17">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>2.84</v>
-      </c>
-      <c r="G17">
-        <v>411</v>
-      </c>
-      <c r="H17">
-        <v>0.02</v>
-      </c>
-      <c r="I17">
-        <v>0.188</v>
-      </c>
-      <c r="J17">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L17">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N17">
-        <v>4</v>
-      </c>
-      <c r="O17">
-        <v>0.16</v>
-      </c>
-      <c r="P17">
-        <v>0.6</v>
-      </c>
-      <c r="Q17">
-        <v>1.6</v>
-      </c>
-      <c r="R17">
-        <v>0.92</v>
-      </c>
-      <c r="S17">
-        <v>3.2</v>
-      </c>
-      <c r="T17">
-        <v>95</v>
-      </c>
-      <c r="U17">
-        <v>66</v>
-      </c>
-      <c r="V17">
-        <v>58</v>
-      </c>
-      <c r="W17">
-        <v>7</v>
-      </c>
-      <c r="X17">
-        <v>0.1</v>
-      </c>
-      <c r="Y17">
-        <v>0.24</v>
-      </c>
-      <c r="Z17">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB17">
-        <v>3</v>
-      </c>
-      <c r="AC17">
-        <v>27</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>61</v>
+        <v>357</v>
       </c>
       <c r="C18">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>1.5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B19">
-        <v>429</v>
+        <v>379</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>72.8</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3.38</v>
       </c>
       <c r="F19">
-        <v>7.14</v>
-      </c>
-      <c r="U19">
-        <v>143</v>
+        <v>7.95</v>
       </c>
       <c r="AC19">
-        <v>36</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B20">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>3.2</v>
+        <v>0.3</v>
       </c>
       <c r="D20">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="E20">
-        <v>4.9000000000000004</v>
+        <v>3.6</v>
       </c>
       <c r="F20">
-        <v>3.27</v>
-      </c>
-      <c r="G20">
-        <v>32</v>
-      </c>
-      <c r="H20">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I20">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J20">
-        <v>0.105</v>
-      </c>
-      <c r="L20">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="O20">
-        <v>0.54</v>
-      </c>
-      <c r="R20">
-        <v>0.05</v>
-      </c>
-      <c r="S20">
-        <v>0.3</v>
-      </c>
-      <c r="T20">
-        <v>150</v>
-      </c>
-      <c r="U20">
-        <v>123</v>
-      </c>
-      <c r="V20">
-        <v>101</v>
-      </c>
-      <c r="W20">
-        <v>12</v>
-      </c>
-      <c r="Y20">
-        <v>0.41</v>
-      </c>
-      <c r="Z20">
-        <v>1E-3</v>
-      </c>
-      <c r="AB20">
         <v>1.9</v>
-      </c>
-      <c r="AC20">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B21">
-        <v>884</v>
+        <v>655</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>69.61</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1751,607 +1655,821 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>14.4</v>
-      </c>
-      <c r="S21">
-        <v>60.2</v>
-      </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="X21">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="AC21">
-        <v>2</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>36</v>
+        <v>340</v>
       </c>
       <c r="C22">
-        <v>0.13</v>
+        <v>36.1</v>
       </c>
       <c r="D22">
-        <v>7.68</v>
+        <v>2.9</v>
       </c>
       <c r="E22">
-        <v>5.76</v>
+        <v>2.9</v>
       </c>
       <c r="F22">
-        <v>0.89</v>
+        <v>2.84</v>
+      </c>
+      <c r="G22">
+        <v>411</v>
+      </c>
+      <c r="H22">
+        <v>0.02</v>
+      </c>
+      <c r="I22">
+        <v>0.188</v>
+      </c>
+      <c r="J22">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22">
+        <v>0.16</v>
+      </c>
+      <c r="P22">
+        <v>0.6</v>
+      </c>
+      <c r="Q22">
+        <v>1.6</v>
+      </c>
+      <c r="R22">
+        <v>0.92</v>
+      </c>
+      <c r="S22">
+        <v>3.2</v>
+      </c>
+      <c r="T22">
+        <v>95</v>
+      </c>
+      <c r="U22">
+        <v>66</v>
+      </c>
+      <c r="V22">
+        <v>58</v>
+      </c>
+      <c r="W22">
+        <v>7</v>
+      </c>
+      <c r="X22">
+        <v>0.1</v>
+      </c>
+      <c r="Y22">
+        <v>0.24</v>
+      </c>
+      <c r="Z22">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB22">
+        <v>3</v>
+      </c>
+      <c r="AC22">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B23">
-        <v>371</v>
+        <v>61</v>
       </c>
       <c r="C23">
-        <v>1.51</v>
+        <v>0.3</v>
       </c>
       <c r="D23">
-        <v>74.67</v>
+        <v>14</v>
       </c>
       <c r="E23">
-        <v>2.7</v>
+        <v>3.9</v>
       </c>
       <c r="F23">
-        <v>13.04</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J23">
-        <v>5.36</v>
-      </c>
-      <c r="X23">
-        <v>3.21</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B24">
-        <v>673</v>
+        <v>429</v>
       </c>
       <c r="C24">
-        <v>68.400000000000006</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>13.1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>3.59</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>13.7</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="I24">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="J24">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="K24">
-        <v>0.313</v>
-      </c>
-      <c r="L24">
-        <v>9.4E-2</v>
-      </c>
-      <c r="N24">
-        <v>34</v>
-      </c>
-      <c r="P24">
-        <v>0.8</v>
-      </c>
-      <c r="R24">
-        <v>9.33</v>
-      </c>
-      <c r="S24">
-        <v>53.9</v>
-      </c>
-      <c r="T24">
-        <v>597</v>
+        <v>7.14</v>
       </c>
       <c r="U24">
-        <v>16</v>
-      </c>
-      <c r="V24">
-        <v>575</v>
-      </c>
-      <c r="W24">
-        <v>251</v>
-      </c>
-      <c r="X24">
-        <v>5.53</v>
-      </c>
-      <c r="Y24">
-        <v>6.45</v>
-      </c>
-      <c r="Z24">
-        <v>1.32</v>
-      </c>
-      <c r="AA24">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AB24">
-        <v>0.7</v>
+        <v>143</v>
       </c>
       <c r="AC24">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B25">
-        <v>263</v>
+        <v>61</v>
       </c>
       <c r="C25">
-        <v>21.2</v>
+        <v>3.2</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F25">
-        <v>16.899999999999999</v>
+        <v>3.27</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="H25">
-        <v>0.73199999999999998</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="I25">
-        <v>0.23499999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="J25">
-        <v>4.34</v>
-      </c>
-      <c r="K25">
-        <v>0.66800000000000004</v>
+        <v>0.105</v>
       </c>
       <c r="L25">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N25">
-        <v>5</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="O25">
-        <v>0.7</v>
-      </c>
-      <c r="P25">
-        <v>0.7</v>
+        <v>0.54</v>
+      </c>
+      <c r="R25">
+        <v>0.05</v>
+      </c>
+      <c r="S25">
+        <v>0.3</v>
       </c>
       <c r="T25">
-        <v>287</v>
+        <v>150</v>
       </c>
       <c r="U25">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="V25">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="W25">
-        <v>19</v>
-      </c>
-      <c r="X25">
-        <v>0.88</v>
+        <v>12</v>
       </c>
       <c r="Y25">
-        <v>2.2000000000000002</v>
+        <v>0.41</v>
       </c>
       <c r="Z25">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA25">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="AB25">
-        <v>24.6</v>
+        <v>1.9</v>
       </c>
       <c r="AC25">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B26">
-        <v>72</v>
+        <v>884</v>
       </c>
       <c r="C26">
-        <v>0.26</v>
+        <v>100</v>
       </c>
       <c r="D26">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>1.81</v>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>14.4</v>
+      </c>
+      <c r="S26">
+        <v>60.2</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC26">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C27">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>7.68</v>
       </c>
       <c r="E27">
-        <v>2.8</v>
+        <v>5.76</v>
       </c>
       <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>426</v>
-      </c>
-      <c r="H27">
-        <v>0.05</v>
-      </c>
-      <c r="I27">
-        <v>0.11</v>
-      </c>
-      <c r="J27">
-        <v>0.6</v>
-      </c>
-      <c r="K27">
-        <v>0.29799999999999999</v>
-      </c>
-      <c r="L27">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="N27">
-        <v>16</v>
-      </c>
-      <c r="P27">
-        <v>9</v>
-      </c>
-      <c r="R27">
-        <v>1.06</v>
-      </c>
-      <c r="S27">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T27">
-        <v>340</v>
-      </c>
-      <c r="U27">
-        <v>21</v>
-      </c>
-      <c r="V27">
-        <v>44</v>
-      </c>
-      <c r="W27">
-        <v>12</v>
-      </c>
-      <c r="X27">
-        <v>0.8</v>
-      </c>
-      <c r="Y27">
-        <v>0.32</v>
-      </c>
-      <c r="Z27">
-        <v>0.127</v>
-      </c>
-      <c r="AA27">
-        <v>0.125</v>
-      </c>
-      <c r="AB27">
-        <v>0.3</v>
-      </c>
-      <c r="AC27">
-        <v>1</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B28">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="C28">
-        <v>1.3</v>
+        <v>1.51</v>
       </c>
       <c r="D28">
-        <v>79.8</v>
+        <v>74.67</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="F28">
-        <v>6.94</v>
+        <v>13.04</v>
       </c>
       <c r="H28">
-        <v>0.16300000000000001</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>1.2999999999999999E-2</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J28">
-        <v>1.48</v>
-      </c>
-      <c r="K28">
-        <v>0.39</v>
-      </c>
-      <c r="L28">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N28">
-        <v>97</v>
-      </c>
-      <c r="R28">
-        <v>0.04</v>
-      </c>
-      <c r="T28">
-        <v>35</v>
-      </c>
-      <c r="U28">
-        <v>10</v>
-      </c>
-      <c r="V28">
-        <v>43</v>
-      </c>
-      <c r="W28">
-        <v>12</v>
+        <v>5.36</v>
       </c>
       <c r="X28">
-        <v>1.2</v>
-      </c>
-      <c r="Y28">
-        <v>0.49</v>
-      </c>
-      <c r="Z28">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="AA28">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="AB28">
-        <v>7.5</v>
-      </c>
-      <c r="AC28">
-        <v>1</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B29">
-        <v>367</v>
+        <v>673</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D29">
-        <v>77</v>
+        <v>13.1</v>
       </c>
       <c r="E29">
-        <v>40</v>
+        <v>3.59</v>
       </c>
       <c r="F29">
-        <v>7</v>
+        <v>13.7</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I29">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J29">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K29">
+        <v>0.313</v>
+      </c>
+      <c r="L29">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N29">
+        <v>34</v>
+      </c>
+      <c r="P29">
+        <v>0.8</v>
+      </c>
+      <c r="R29">
+        <v>9.33</v>
+      </c>
+      <c r="S29">
+        <v>53.9</v>
       </c>
       <c r="T29">
-        <v>106</v>
+        <v>597</v>
       </c>
       <c r="U29">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="V29">
+        <v>575</v>
+      </c>
+      <c r="W29">
+        <v>251</v>
       </c>
       <c r="X29">
-        <v>1.0900000000000001</v>
+        <v>5.53</v>
+      </c>
+      <c r="Y29">
+        <v>6.45</v>
+      </c>
+      <c r="Z29">
+        <v>1.32</v>
+      </c>
+      <c r="AA29">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AB29">
+        <v>0.7</v>
       </c>
       <c r="AC29">
-        <v>106</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B30">
-        <v>36</v>
+        <v>263</v>
       </c>
       <c r="C30">
-        <v>0.22</v>
+        <v>21.2</v>
       </c>
       <c r="D30">
-        <v>7.96</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>4.8600000000000003</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0.64</v>
-      </c>
-      <c r="M30">
-        <v>3.7</v>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="I30">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="J30">
+        <v>4.34</v>
+      </c>
+      <c r="K30">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="L30">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="N30">
+        <v>5</v>
+      </c>
+      <c r="O30">
+        <v>0.7</v>
       </c>
       <c r="P30">
-        <v>59.6</v>
+        <v>0.7</v>
       </c>
       <c r="T30">
-        <v>161</v>
+        <v>287</v>
       </c>
       <c r="U30">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="V30">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="W30">
-        <v>12.5</v>
+        <v>19</v>
       </c>
       <c r="X30">
-        <v>0.26</v>
+        <v>0.88</v>
       </c>
       <c r="Y30">
-        <v>0.11</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z30">
-        <v>3.5000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA30">
-        <v>0.36799999999999999</v>
+        <v>0.01</v>
+      </c>
+      <c r="AB30">
+        <v>24.6</v>
       </c>
       <c r="AC30">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B31">
-        <v>385</v>
+        <v>72</v>
       </c>
       <c r="C31">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="D31">
-        <v>99.7</v>
+        <v>16</v>
       </c>
       <c r="E31">
-        <v>99.7</v>
+        <v>0.65</v>
       </c>
       <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>1.9E-2</v>
-      </c>
-      <c r="T31">
-        <v>2</v>
-      </c>
-      <c r="U31">
-        <v>1</v>
-      </c>
-      <c r="X31">
-        <v>0.05</v>
-      </c>
-      <c r="Y31">
-        <v>0.01</v>
-      </c>
-      <c r="Z31">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB31">
-        <v>0.6</v>
-      </c>
-      <c r="AC31">
-        <v>1</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>2.8</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>426</v>
+      </c>
+      <c r="H32">
+        <v>0.05</v>
+      </c>
+      <c r="I32">
+        <v>0.11</v>
+      </c>
+      <c r="J32">
+        <v>0.6</v>
+      </c>
+      <c r="K32">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="L32">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N32">
+        <v>16</v>
+      </c>
+      <c r="P32">
+        <v>9</v>
+      </c>
+      <c r="R32">
+        <v>1.06</v>
+      </c>
+      <c r="S32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T32">
+        <v>340</v>
+      </c>
+      <c r="U32">
+        <v>21</v>
+      </c>
+      <c r="V32">
+        <v>44</v>
+      </c>
+      <c r="W32">
+        <v>12</v>
+      </c>
+      <c r="X32">
+        <v>0.8</v>
+      </c>
+      <c r="Y32">
+        <v>0.32</v>
+      </c>
+      <c r="Z32">
+        <v>0.127</v>
+      </c>
+      <c r="AA32">
+        <v>0.125</v>
+      </c>
+      <c r="AB32">
+        <v>0.3</v>
+      </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>359</v>
+      </c>
+      <c r="C33">
+        <v>1.3</v>
+      </c>
+      <c r="D33">
+        <v>79.8</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>6.94</v>
+      </c>
+      <c r="H33">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I33">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J33">
+        <v>1.48</v>
+      </c>
+      <c r="K33">
+        <v>0.39</v>
+      </c>
+      <c r="L33">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N33">
+        <v>97</v>
+      </c>
+      <c r="R33">
+        <v>0.04</v>
+      </c>
+      <c r="T33">
+        <v>35</v>
+      </c>
+      <c r="U33">
+        <v>10</v>
+      </c>
+      <c r="V33">
+        <v>43</v>
+      </c>
+      <c r="W33">
+        <v>12</v>
+      </c>
+      <c r="X33">
+        <v>1.2</v>
+      </c>
+      <c r="Y33">
+        <v>0.49</v>
+      </c>
+      <c r="Z33">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AA33">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB33">
+        <v>7.5</v>
+      </c>
+      <c r="AC33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34">
+        <v>367</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>77</v>
+      </c>
+      <c r="E34">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>7</v>
+      </c>
+      <c r="T34">
+        <v>106</v>
+      </c>
+      <c r="U34">
+        <v>30</v>
+      </c>
+      <c r="X34">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AC34">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>0.22</v>
+      </c>
+      <c r="D35">
+        <v>7.96</v>
+      </c>
+      <c r="E35">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="F35">
+        <v>0.64</v>
+      </c>
+      <c r="M35">
+        <v>3.7</v>
+      </c>
+      <c r="P35">
+        <v>59.6</v>
+      </c>
+      <c r="T35">
+        <v>161</v>
+      </c>
+      <c r="U35">
+        <v>17</v>
+      </c>
+      <c r="V35">
+        <v>23</v>
+      </c>
+      <c r="W35">
+        <v>12.5</v>
+      </c>
+      <c r="X35">
+        <v>0.26</v>
+      </c>
+      <c r="Y35">
+        <v>0.11</v>
+      </c>
+      <c r="Z35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA35">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AC35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>385</v>
+      </c>
+      <c r="C36">
+        <v>0.32</v>
+      </c>
+      <c r="D36">
+        <v>99.7</v>
+      </c>
+      <c r="E36">
+        <v>99.7</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T36">
+        <v>2</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>0.05</v>
+      </c>
+      <c r="Y36">
+        <v>0.01</v>
+      </c>
+      <c r="Z36">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB36">
+        <v>0.6</v>
+      </c>
+      <c r="AC36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B32">
+      <c r="B37">
         <v>18</v>
       </c>
-      <c r="C32">
+      <c r="C37">
         <v>0.2</v>
       </c>
-      <c r="D32">
+      <c r="D37">
         <v>3.9</v>
       </c>
-      <c r="E32">
+      <c r="E37">
         <v>2.6</v>
       </c>
-      <c r="F32">
+      <c r="F37">
         <v>0.9</v>
       </c>
-      <c r="G32">
+      <c r="G37">
         <v>42</v>
       </c>
-      <c r="H32">
+      <c r="H37">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="I32">
+      <c r="I37">
         <v>1.9E-2</v>
       </c>
-      <c r="J32">
+      <c r="J37">
         <v>0.59399999999999997</v>
       </c>
-      <c r="K32">
+      <c r="K37">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="L32">
+      <c r="L37">
         <v>0.08</v>
       </c>
-      <c r="N32">
+      <c r="N37">
         <v>15</v>
       </c>
-      <c r="P32">
+      <c r="P37">
         <v>13.7</v>
       </c>
-      <c r="R32">
+      <c r="R37">
         <v>0.54</v>
       </c>
-      <c r="S32">
+      <c r="S37">
         <v>7.9</v>
       </c>
-      <c r="T32">
+      <c r="T37">
         <v>237</v>
       </c>
-      <c r="U32">
+      <c r="U37">
         <v>10</v>
       </c>
-      <c r="V32">
+      <c r="V37">
         <v>24</v>
       </c>
-      <c r="W32">
+      <c r="W37">
         <v>11</v>
       </c>
-      <c r="X32">
+      <c r="X37">
         <v>0.27</v>
       </c>
-      <c r="Y32">
+      <c r="Y37">
         <v>0.17</v>
       </c>
-      <c r="Z32">
+      <c r="Z37">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AC32">
+      <c r="AC37">
         <v>5</v>
       </c>
     </row>
@@ -2416,7 +2534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G33:G1048576 H32 G1:G31">
+  <conditionalFormatting sqref="G38:G1048576 H37 G1:G36">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2428,7 +2546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:H1048576 I32 H1:H31">
+  <conditionalFormatting sqref="H38:H1048576 I37 H1:H36">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2440,7 +2558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I1048576 J32 I1:I31">
+  <conditionalFormatting sqref="I38:I1048576 J37 I1:I36">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2452,7 +2570,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33:J1048576 J1:J31">
+  <conditionalFormatting sqref="J38:J1048576 J1:J36">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
amaretti and some changes
</commit_message>
<xml_diff>
--- a/data/foodProperties.xlsx
+++ b/data/foodProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1pab\Desktop\Pablo\showtime\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E555EDCF-04B4-42B7-A588-7918C6A51B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED7E4CB-37F8-4C4F-9468-5257A3D830E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Ingredient</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>cob of corn</t>
+  </si>
+  <si>
+    <t>almond</t>
+  </si>
+  <si>
+    <t>banana</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,76 +874,67 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>622</v>
       </c>
       <c r="C4">
-        <v>0.17</v>
+        <v>50.2</v>
       </c>
       <c r="D4">
-        <v>13.8</v>
+        <v>16.2</v>
       </c>
       <c r="E4">
-        <v>10.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F4">
-        <v>0.26</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
+        <v>26.2</v>
       </c>
       <c r="H4">
-        <v>1.7000000000000001E-2</v>
+        <v>0.112</v>
       </c>
       <c r="I4">
-        <v>2.5999999999999999E-2</v>
+        <v>0.748</v>
       </c>
       <c r="J4">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="K4">
-        <v>6.0999999999999999E-2</v>
+        <v>4</v>
       </c>
       <c r="L4">
-        <v>4.1000000000000002E-2</v>
+        <v>0.1</v>
+      </c>
+      <c r="M4">
+        <v>69.099999999999994</v>
       </c>
       <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="R4">
-        <v>0.18</v>
-      </c>
-      <c r="S4">
-        <v>2.2000000000000002</v>
+        <v>38</v>
       </c>
       <c r="T4">
-        <v>107</v>
+        <v>667</v>
       </c>
       <c r="U4">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="V4">
-        <v>11</v>
+        <v>512</v>
       </c>
       <c r="W4">
-        <v>5</v>
+        <v>251</v>
       </c>
       <c r="X4">
-        <v>0.12</v>
+        <v>3.22</v>
       </c>
       <c r="Y4">
-        <v>0.04</v>
+        <v>2.8</v>
       </c>
       <c r="Z4">
-        <v>2.7E-2</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="AA4">
-        <v>3.5000000000000003E-2</v>
+        <v>1.81</v>
+      </c>
+      <c r="AB4">
+        <v>0.7</v>
       </c>
       <c r="AC4">
         <v>1</v>
@@ -945,922 +942,982 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C5">
-        <v>0.64</v>
+        <v>0.17</v>
       </c>
       <c r="D5">
-        <v>2.65</v>
+        <v>13.8</v>
       </c>
       <c r="E5">
-        <v>0.3</v>
+        <v>10.4</v>
       </c>
       <c r="F5">
-        <v>3.15</v>
+        <v>0.26</v>
       </c>
       <c r="G5">
-        <v>264</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>3.4000000000000002E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I5">
-        <v>7.5999999999999998E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J5">
-        <v>0.90200000000000002</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="K5">
-        <v>0.20899999999999999</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="L5">
-        <v>0.155</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="N5">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="P5">
-        <v>18</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="R5">
-        <v>0.8</v>
+        <v>0.18</v>
       </c>
       <c r="S5">
-        <v>415</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="T5">
-        <v>295</v>
+        <v>107</v>
       </c>
       <c r="U5">
-        <v>177</v>
+        <v>6</v>
       </c>
       <c r="V5">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="W5">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="X5">
-        <v>3.17</v>
+        <v>0.12</v>
       </c>
       <c r="Y5">
-        <v>0.81</v>
+        <v>0.04</v>
       </c>
       <c r="Z5">
-        <v>0.38500000000000001</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AA5">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AB5">
-        <v>0.3</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AC5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B6">
-        <v>254</v>
+        <v>98</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>15.8</v>
       </c>
       <c r="F6">
-        <v>17.2</v>
+        <v>0.74</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>4.2999999999999997E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="I6">
-        <v>0.151</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="K6">
-        <v>0.498</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="L6">
-        <v>0.32300000000000001</v>
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="M6">
+        <v>2E-3</v>
       </c>
       <c r="N6">
-        <v>7</v>
-      </c>
-      <c r="O6">
-        <v>2.14</v>
-      </c>
-      <c r="Q6">
+        <v>14</v>
+      </c>
+      <c r="P6">
+        <v>12.3</v>
+      </c>
+      <c r="S6">
         <v>0.1</v>
       </c>
-      <c r="R6">
-        <v>0.17</v>
-      </c>
-      <c r="S6">
-        <v>1.8</v>
-      </c>
       <c r="T6">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="U6">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="V6">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="W6">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="X6">
-        <v>1.94</v>
+        <v>0.2</v>
       </c>
       <c r="Y6">
-        <v>4.18</v>
+        <v>0.16</v>
       </c>
       <c r="Z6">
-        <v>6.0999999999999999E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="AA6">
-        <v>0.01</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="AB6">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AC6">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>0.16</v>
+        <v>0.64</v>
       </c>
       <c r="D7">
-        <v>6.7</v>
+        <v>2.65</v>
       </c>
       <c r="E7">
-        <v>4.2</v>
+        <v>0.3</v>
       </c>
       <c r="F7">
-        <v>0.88</v>
+        <v>3.15</v>
+      </c>
+      <c r="G7">
+        <v>264</v>
+      </c>
+      <c r="H7">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="K7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.155</v>
+      </c>
+      <c r="N7">
+        <v>68</v>
+      </c>
+      <c r="P7">
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <v>0.8</v>
+      </c>
+      <c r="S7">
+        <v>415</v>
+      </c>
+      <c r="T7">
+        <v>295</v>
+      </c>
+      <c r="U7">
+        <v>177</v>
+      </c>
+      <c r="V7">
+        <v>56</v>
+      </c>
+      <c r="W7">
+        <v>64</v>
+      </c>
+      <c r="X7">
+        <v>3.17</v>
+      </c>
+      <c r="Y7">
+        <v>0.81</v>
+      </c>
+      <c r="Z7">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AA7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AB7">
+        <v>0.3</v>
+      </c>
+      <c r="AC7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>17.2</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.151</v>
+      </c>
+      <c r="J8">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="K8">
+        <v>0.498</v>
+      </c>
+      <c r="L8">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>2.14</v>
+      </c>
+      <c r="Q8">
         <v>0.1</v>
       </c>
-      <c r="D8">
-        <v>5.8</v>
-      </c>
-      <c r="E8">
-        <v>3.2</v>
-      </c>
-      <c r="F8">
-        <v>1.28</v>
+      <c r="R8">
+        <v>0.17</v>
+      </c>
+      <c r="S8">
+        <v>1.8</v>
+      </c>
+      <c r="T8">
+        <v>270</v>
+      </c>
+      <c r="U8">
+        <v>18</v>
+      </c>
+      <c r="V8">
+        <v>158</v>
+      </c>
+      <c r="W8">
+        <v>17</v>
+      </c>
+      <c r="X8">
+        <v>1.94</v>
+      </c>
+      <c r="Y8">
+        <v>4.18</v>
+      </c>
+      <c r="Z8">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AA8">
+        <v>0.01</v>
+      </c>
+      <c r="AB8">
+        <v>15</v>
+      </c>
+      <c r="AC8">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C9">
-        <v>0.35</v>
+        <v>0.16</v>
       </c>
       <c r="D9">
-        <v>10.3</v>
+        <v>6.7</v>
       </c>
       <c r="E9">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="F9">
-        <v>0.94</v>
-      </c>
-      <c r="G9">
-        <v>835</v>
-      </c>
-      <c r="H9">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I9">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="J9">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="K9">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="L9">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="N9">
-        <v>19</v>
-      </c>
-      <c r="P9">
-        <v>5.9</v>
-      </c>
-      <c r="R9">
-        <v>0.66</v>
-      </c>
-      <c r="S9">
-        <v>13.2</v>
-      </c>
-      <c r="T9">
-        <v>320</v>
-      </c>
-      <c r="U9">
-        <v>33</v>
-      </c>
-      <c r="V9">
-        <v>35</v>
-      </c>
-      <c r="W9">
-        <v>12</v>
-      </c>
-      <c r="X9">
-        <v>0.3</v>
-      </c>
-      <c r="Y9">
-        <v>0.24</v>
-      </c>
-      <c r="Z9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA9">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="AB9">
-        <v>0.1</v>
-      </c>
-      <c r="AC9">
-        <v>69</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="D10">
-        <v>2.97</v>
+        <v>5.8</v>
       </c>
       <c r="E10">
-        <v>1.34</v>
+        <v>3.2</v>
       </c>
       <c r="F10">
-        <v>0.69</v>
-      </c>
-      <c r="G10">
-        <v>22</v>
-      </c>
-      <c r="H10">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="I10">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="J10">
-        <v>0.32</v>
-      </c>
-      <c r="K10">
-        <v>0.246</v>
-      </c>
-      <c r="L10">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="N10">
-        <v>36</v>
-      </c>
-      <c r="P10">
-        <v>3.1</v>
-      </c>
-      <c r="R10">
-        <v>0.27</v>
-      </c>
-      <c r="S10">
-        <v>29.3</v>
-      </c>
-      <c r="T10">
-        <v>260</v>
-      </c>
-      <c r="U10">
-        <v>40</v>
-      </c>
-      <c r="V10">
-        <v>24</v>
-      </c>
-      <c r="W10">
-        <v>11</v>
-      </c>
-      <c r="X10">
-        <v>0.2</v>
-      </c>
-      <c r="Y10">
-        <v>0.13</v>
-      </c>
-      <c r="Z10">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="AA10">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="AB10">
-        <v>0.4</v>
-      </c>
-      <c r="AC10">
-        <v>80</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C11">
-        <v>1.93</v>
+        <v>0.35</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>10.3</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="F11">
-        <v>22.5</v>
+        <v>0.94</v>
+      </c>
+      <c r="G11">
+        <v>835</v>
+      </c>
+      <c r="H11">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="I11">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="J11">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="L11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="N11">
+        <v>19</v>
+      </c>
+      <c r="P11">
+        <v>5.9</v>
+      </c>
+      <c r="R11">
+        <v>0.66</v>
+      </c>
+      <c r="S11">
+        <v>13.2</v>
+      </c>
+      <c r="T11">
+        <v>320</v>
+      </c>
+      <c r="U11">
+        <v>33</v>
+      </c>
+      <c r="V11">
+        <v>35</v>
+      </c>
+      <c r="W11">
+        <v>12</v>
+      </c>
+      <c r="X11">
+        <v>0.3</v>
+      </c>
+      <c r="Y11">
+        <v>0.24</v>
+      </c>
+      <c r="Z11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AA11">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AB11">
+        <v>0.1</v>
+      </c>
+      <c r="AC11">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B12">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>1.7</v>
+        <v>0.17</v>
       </c>
       <c r="D12">
-        <v>14.2</v>
+        <v>2.97</v>
       </c>
       <c r="E12">
+        <v>1.34</v>
+      </c>
+      <c r="F12">
+        <v>0.69</v>
+      </c>
+      <c r="G12">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I12">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.32</v>
+      </c>
+      <c r="K12">
+        <v>0.246</v>
+      </c>
+      <c r="L12">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="N12">
+        <v>36</v>
+      </c>
+      <c r="P12">
+        <v>3.1</v>
+      </c>
+      <c r="R12">
+        <v>0.27</v>
+      </c>
+      <c r="S12">
+        <v>29.3</v>
+      </c>
+      <c r="T12">
+        <v>260</v>
+      </c>
+      <c r="U12">
+        <v>40</v>
+      </c>
+      <c r="V12">
+        <v>24</v>
+      </c>
+      <c r="W12">
+        <v>11</v>
+      </c>
+      <c r="X12">
         <v>0.2</v>
       </c>
-      <c r="F12">
-        <v>6.9</v>
+      <c r="Y12">
+        <v>0.13</v>
+      </c>
+      <c r="Z12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA12">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AB12">
+        <v>0.4</v>
+      </c>
+      <c r="AC12">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="B13">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C13">
-        <v>1.35</v>
+        <v>1.93</v>
       </c>
       <c r="D13">
-        <v>18.7</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>6.26</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>3.27</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B14">
-        <v>420</v>
+        <v>109</v>
       </c>
       <c r="C14">
-        <v>27.8</v>
+        <v>1.7</v>
       </c>
       <c r="D14">
-        <v>13.9</v>
+        <v>14.2</v>
       </c>
       <c r="E14">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="F14">
-        <v>28.4</v>
-      </c>
-      <c r="G14">
-        <v>262</v>
-      </c>
-      <c r="H14">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="I14">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="J14">
-        <v>0.08</v>
-      </c>
-      <c r="K14">
-        <v>0.45</v>
-      </c>
-      <c r="L14">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="N14">
-        <v>6</v>
-      </c>
-      <c r="O14">
-        <v>1.4</v>
-      </c>
-      <c r="Q14">
-        <v>0.5</v>
-      </c>
-      <c r="R14">
-        <v>0.53</v>
-      </c>
-      <c r="S14">
-        <v>1.7</v>
-      </c>
-      <c r="T14">
-        <v>180</v>
-      </c>
-      <c r="U14">
-        <v>853</v>
-      </c>
-      <c r="V14">
-        <v>627</v>
-      </c>
-      <c r="W14">
-        <v>34</v>
-      </c>
-      <c r="X14">
-        <v>0.49</v>
-      </c>
-      <c r="Y14">
-        <v>4.2</v>
-      </c>
-      <c r="Z14">
-        <v>0.04</v>
-      </c>
-      <c r="AA14">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="AB14">
-        <v>34.4</v>
-      </c>
-      <c r="AC14">
-        <v>1800</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B15">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="C15">
-        <v>9.9600000000000009</v>
+        <v>1.35</v>
       </c>
       <c r="D15">
-        <v>0.96</v>
+        <v>18.7</v>
       </c>
       <c r="E15">
-        <v>0.2</v>
+        <v>6.26</v>
       </c>
       <c r="F15">
-        <v>12.4</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B16">
-        <v>322</v>
+        <v>420</v>
       </c>
       <c r="C16">
-        <v>26.5</v>
+        <v>27.8</v>
       </c>
       <c r="D16">
-        <v>3.59</v>
+        <v>13.9</v>
       </c>
       <c r="E16">
-        <v>0.56000000000000005</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F16">
-        <v>15.9</v>
+        <v>28.4</v>
       </c>
       <c r="G16">
-        <v>381</v>
+        <v>262</v>
       </c>
       <c r="H16">
-        <v>0.17599999999999999</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I16">
-        <v>0.52800000000000002</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="J16">
-        <v>2.4E-2</v>
+        <v>0.08</v>
       </c>
       <c r="K16">
-        <v>2.99</v>
+        <v>0.45</v>
       </c>
       <c r="L16">
-        <v>0.35</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="N16">
-        <v>146</v>
+        <v>6</v>
       </c>
       <c r="O16">
-        <v>1.95</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="Q16">
-        <v>5.4</v>
+        <v>0.5</v>
       </c>
       <c r="R16">
-        <v>2.58</v>
+        <v>0.53</v>
       </c>
       <c r="S16">
-        <v>0.7</v>
+        <v>1.7</v>
       </c>
       <c r="T16">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="U16">
-        <v>129</v>
+        <v>853</v>
       </c>
       <c r="V16">
-        <v>390</v>
+        <v>627</v>
       </c>
       <c r="W16">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="X16">
-        <v>2.73</v>
+        <v>0.49</v>
       </c>
       <c r="Y16">
-        <v>2.2999999999999998</v>
+        <v>4.2</v>
       </c>
       <c r="Z16">
-        <v>7.6999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AA16">
-        <v>5.5E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="AB16">
-        <v>56</v>
+        <v>34.4</v>
       </c>
       <c r="AC16">
-        <v>48</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17">
-        <v>0.38</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D17">
-        <v>28.2</v>
+        <v>0.96</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F17">
-        <v>6.62</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="C18">
+        <v>26.5</v>
+      </c>
+      <c r="D18">
+        <v>3.59</v>
+      </c>
+      <c r="E18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F18">
+        <v>15.9</v>
+      </c>
+      <c r="G18">
+        <v>381</v>
+      </c>
+      <c r="H18">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I18">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K18">
+        <v>2.99</v>
+      </c>
+      <c r="L18">
+        <v>0.35</v>
+      </c>
+      <c r="N18">
+        <v>146</v>
+      </c>
+      <c r="O18">
+        <v>1.95</v>
+      </c>
+      <c r="P18">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>89</v>
+      <c r="Q18">
+        <v>5.4</v>
+      </c>
+      <c r="R18">
+        <v>2.58</v>
+      </c>
+      <c r="S18">
+        <v>0.7</v>
+      </c>
+      <c r="T18">
+        <v>109</v>
+      </c>
+      <c r="U18">
+        <v>129</v>
+      </c>
+      <c r="V18">
+        <v>390</v>
+      </c>
+      <c r="W18">
+        <v>5</v>
+      </c>
+      <c r="X18">
+        <v>2.73</v>
+      </c>
+      <c r="Y18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z18">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AA18">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AB18">
+        <v>56</v>
+      </c>
+      <c r="AC18">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B19">
-        <v>379</v>
+        <v>143</v>
       </c>
       <c r="C19">
-        <v>4.4000000000000004</v>
+        <v>0.38</v>
       </c>
       <c r="D19">
-        <v>72.8</v>
+        <v>28.2</v>
       </c>
       <c r="E19">
-        <v>3.38</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>7.95</v>
-      </c>
-      <c r="AC19">
-        <v>0.49</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="B20">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C20">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>1.9</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B21">
-        <v>655</v>
+        <v>379</v>
       </c>
       <c r="C21">
-        <v>69.61</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>72.8</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>3.38</v>
       </c>
       <c r="F21">
-        <v>6.38</v>
+        <v>7.95</v>
+      </c>
+      <c r="AC21">
+        <v>0.49</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B22">
-        <v>340</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>36.1</v>
+        <v>0.3</v>
       </c>
       <c r="D22">
-        <v>2.9</v>
+        <v>7.9</v>
       </c>
       <c r="E22">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="F22">
-        <v>2.84</v>
-      </c>
-      <c r="G22">
-        <v>411</v>
-      </c>
-      <c r="H22">
-        <v>0.02</v>
-      </c>
-      <c r="I22">
-        <v>0.188</v>
-      </c>
-      <c r="J22">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="L22">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="N22">
-        <v>4</v>
-      </c>
-      <c r="O22">
-        <v>0.16</v>
-      </c>
-      <c r="P22">
-        <v>0.6</v>
-      </c>
-      <c r="Q22">
-        <v>1.6</v>
-      </c>
-      <c r="R22">
-        <v>0.92</v>
-      </c>
-      <c r="S22">
-        <v>3.2</v>
-      </c>
-      <c r="T22">
-        <v>95</v>
-      </c>
-      <c r="U22">
-        <v>66</v>
-      </c>
-      <c r="V22">
-        <v>58</v>
-      </c>
-      <c r="W22">
-        <v>7</v>
-      </c>
-      <c r="X22">
-        <v>0.1</v>
-      </c>
-      <c r="Y22">
-        <v>0.24</v>
-      </c>
-      <c r="Z22">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="AB22">
-        <v>3</v>
-      </c>
-      <c r="AC22">
-        <v>27</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B23">
-        <v>61</v>
+        <v>655</v>
       </c>
       <c r="C23">
-        <v>0.3</v>
+        <v>69.61</v>
       </c>
       <c r="D23">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>1.5</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24">
-        <v>429</v>
+        <v>340</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>36.1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="F24">
-        <v>7.14</v>
+        <v>2.84</v>
+      </c>
+      <c r="G24">
+        <v>411</v>
+      </c>
+      <c r="H24">
+        <v>0.02</v>
+      </c>
+      <c r="I24">
+        <v>0.188</v>
+      </c>
+      <c r="J24">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L24">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>0.16</v>
+      </c>
+      <c r="P24">
+        <v>0.6</v>
+      </c>
+      <c r="Q24">
+        <v>1.6</v>
+      </c>
+      <c r="R24">
+        <v>0.92</v>
+      </c>
+      <c r="S24">
+        <v>3.2</v>
+      </c>
+      <c r="T24">
+        <v>95</v>
       </c>
       <c r="U24">
-        <v>143</v>
+        <v>66</v>
+      </c>
+      <c r="V24">
+        <v>58</v>
+      </c>
+      <c r="W24">
+        <v>7</v>
+      </c>
+      <c r="X24">
+        <v>0.1</v>
+      </c>
+      <c r="Y24">
+        <v>0.24</v>
+      </c>
+      <c r="Z24">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AB24">
+        <v>3</v>
       </c>
       <c r="AC24">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>61</v>
       </c>
       <c r="C25">
-        <v>3.2</v>
+        <v>0.3</v>
       </c>
       <c r="D25">
-        <v>4.9000000000000004</v>
+        <v>14</v>
       </c>
       <c r="E25">
-        <v>4.9000000000000004</v>
+        <v>3.9</v>
       </c>
       <c r="F25">
-        <v>3.27</v>
-      </c>
-      <c r="G25">
-        <v>32</v>
-      </c>
-      <c r="H25">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I25">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="J25">
-        <v>0.105</v>
-      </c>
-      <c r="L25">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="O25">
-        <v>0.54</v>
-      </c>
-      <c r="R25">
-        <v>0.05</v>
-      </c>
-      <c r="S25">
-        <v>0.3</v>
-      </c>
-      <c r="T25">
-        <v>150</v>
-      </c>
-      <c r="U25">
-        <v>123</v>
-      </c>
-      <c r="V25">
-        <v>101</v>
-      </c>
-      <c r="W25">
-        <v>12</v>
-      </c>
-      <c r="Y25">
-        <v>0.41</v>
-      </c>
-      <c r="Z25">
-        <v>1E-3</v>
-      </c>
-      <c r="AB25">
-        <v>1.9</v>
-      </c>
-      <c r="AC25">
-        <v>38</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26">
-        <v>884</v>
+        <v>429</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1869,607 +1926,701 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>14.4</v>
-      </c>
-      <c r="S26">
-        <v>60.2</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
+        <v>7.14</v>
       </c>
       <c r="U26">
-        <v>1</v>
-      </c>
-      <c r="X26">
-        <v>0.56000000000000005</v>
+        <v>143</v>
       </c>
       <c r="AC26">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C27">
-        <v>0.13</v>
+        <v>3.2</v>
       </c>
       <c r="D27">
-        <v>7.68</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E27">
-        <v>5.76</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F27">
-        <v>0.89</v>
+        <v>3.27</v>
+      </c>
+      <c r="G27">
+        <v>32</v>
+      </c>
+      <c r="H27">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I27">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J27">
+        <v>0.105</v>
+      </c>
+      <c r="L27">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O27">
+        <v>0.54</v>
+      </c>
+      <c r="R27">
+        <v>0.05</v>
+      </c>
+      <c r="S27">
+        <v>0.3</v>
+      </c>
+      <c r="T27">
+        <v>150</v>
+      </c>
+      <c r="U27">
+        <v>123</v>
+      </c>
+      <c r="V27">
+        <v>101</v>
+      </c>
+      <c r="W27">
+        <v>12</v>
+      </c>
+      <c r="Y27">
+        <v>0.41</v>
+      </c>
+      <c r="Z27">
+        <v>1E-3</v>
+      </c>
+      <c r="AB27">
+        <v>1.9</v>
+      </c>
+      <c r="AC27">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28">
-        <v>371</v>
+        <v>884</v>
       </c>
       <c r="C28">
-        <v>1.51</v>
+        <v>100</v>
       </c>
       <c r="D28">
-        <v>74.67</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>13.04</v>
-      </c>
-      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>14.4</v>
+      </c>
+      <c r="S28">
+        <v>60.2</v>
+      </c>
+      <c r="T28">
         <v>1</v>
       </c>
-      <c r="I28">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="J28">
-        <v>5.36</v>
+      <c r="U28">
+        <v>1</v>
       </c>
       <c r="X28">
-        <v>3.21</v>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B29">
-        <v>673</v>
+        <v>36</v>
       </c>
       <c r="C29">
-        <v>68.400000000000006</v>
+        <v>0.13</v>
       </c>
       <c r="D29">
-        <v>13.1</v>
+        <v>7.68</v>
       </c>
       <c r="E29">
-        <v>3.59</v>
+        <v>5.76</v>
       </c>
       <c r="F29">
-        <v>13.7</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="I29">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="J29">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="K29">
-        <v>0.313</v>
-      </c>
-      <c r="L29">
-        <v>9.4E-2</v>
-      </c>
-      <c r="N29">
-        <v>34</v>
-      </c>
-      <c r="P29">
-        <v>0.8</v>
-      </c>
-      <c r="R29">
-        <v>9.33</v>
-      </c>
-      <c r="S29">
-        <v>53.9</v>
-      </c>
-      <c r="T29">
-        <v>597</v>
-      </c>
-      <c r="U29">
-        <v>16</v>
-      </c>
-      <c r="V29">
-        <v>575</v>
-      </c>
-      <c r="W29">
-        <v>251</v>
-      </c>
-      <c r="X29">
-        <v>5.53</v>
-      </c>
-      <c r="Y29">
-        <v>6.45</v>
-      </c>
-      <c r="Z29">
-        <v>1.32</v>
-      </c>
-      <c r="AA29">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AB29">
-        <v>0.7</v>
-      </c>
-      <c r="AC29">
-        <v>2</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B30">
-        <v>263</v>
+        <v>371</v>
       </c>
       <c r="C30">
-        <v>21.2</v>
+        <v>1.51</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>74.67</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="F30">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
+        <v>13.04</v>
       </c>
       <c r="H30">
-        <v>0.73199999999999998</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>0.23499999999999999</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="J30">
-        <v>4.34</v>
-      </c>
-      <c r="K30">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L30">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="N30">
-        <v>5</v>
-      </c>
-      <c r="O30">
-        <v>0.7</v>
-      </c>
-      <c r="P30">
-        <v>0.7</v>
-      </c>
-      <c r="T30">
-        <v>287</v>
-      </c>
-      <c r="U30">
-        <v>14</v>
-      </c>
-      <c r="V30">
-        <v>175</v>
-      </c>
-      <c r="W30">
-        <v>19</v>
+        <v>5.36</v>
       </c>
       <c r="X30">
-        <v>0.88</v>
-      </c>
-      <c r="Y30">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Z30">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AA30">
-        <v>0.01</v>
-      </c>
-      <c r="AB30">
-        <v>24.6</v>
-      </c>
-      <c r="AC30">
-        <v>56</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B31">
-        <v>72</v>
+        <v>673</v>
       </c>
       <c r="C31">
-        <v>0.26</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D31">
+        <v>13.1</v>
+      </c>
+      <c r="E31">
+        <v>3.59</v>
+      </c>
+      <c r="F31">
+        <v>13.7</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="I31">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J31">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K31">
+        <v>0.313</v>
+      </c>
+      <c r="L31">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N31">
+        <v>34</v>
+      </c>
+      <c r="P31">
+        <v>0.8</v>
+      </c>
+      <c r="R31">
+        <v>9.33</v>
+      </c>
+      <c r="S31">
+        <v>53.9</v>
+      </c>
+      <c r="T31">
+        <v>597</v>
+      </c>
+      <c r="U31">
         <v>16</v>
       </c>
-      <c r="E31">
-        <v>0.65</v>
-      </c>
-      <c r="F31">
-        <v>1.81</v>
+      <c r="V31">
+        <v>575</v>
+      </c>
+      <c r="W31">
+        <v>251</v>
+      </c>
+      <c r="X31">
+        <v>5.53</v>
+      </c>
+      <c r="Y31">
+        <v>6.45</v>
+      </c>
+      <c r="Z31">
+        <v>1.32</v>
+      </c>
+      <c r="AA31">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AB31">
+        <v>0.7</v>
+      </c>
+      <c r="AC31">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B32">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="C32">
-        <v>0.1</v>
+        <v>21.2</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="G32">
-        <v>426</v>
+        <v>2</v>
       </c>
       <c r="H32">
-        <v>0.05</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="I32">
-        <v>0.11</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="J32">
-        <v>0.6</v>
+        <v>4.34</v>
       </c>
       <c r="K32">
-        <v>0.29799999999999999</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="L32">
-        <v>6.0999999999999999E-2</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="N32">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="O32">
+        <v>0.7</v>
       </c>
       <c r="P32">
-        <v>9</v>
-      </c>
-      <c r="R32">
-        <v>1.06</v>
-      </c>
-      <c r="S32">
-        <v>1.1000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="T32">
-        <v>340</v>
+        <v>287</v>
       </c>
       <c r="U32">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V32">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="W32">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X32">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="Y32">
-        <v>0.32</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z32">
-        <v>0.127</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AA32">
-        <v>0.125</v>
+        <v>0.01</v>
       </c>
       <c r="AB32">
-        <v>0.3</v>
+        <v>24.6</v>
       </c>
       <c r="AC32">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33">
-        <v>359</v>
+        <v>72</v>
       </c>
       <c r="C33">
-        <v>1.3</v>
+        <v>0.26</v>
       </c>
       <c r="D33">
-        <v>79.8</v>
+        <v>16</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F33">
-        <v>6.94</v>
-      </c>
-      <c r="H33">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="I33">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="J33">
-        <v>1.48</v>
-      </c>
-      <c r="K33">
-        <v>0.39</v>
-      </c>
-      <c r="L33">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N33">
-        <v>97</v>
-      </c>
-      <c r="R33">
-        <v>0.04</v>
-      </c>
-      <c r="T33">
-        <v>35</v>
-      </c>
-      <c r="U33">
-        <v>10</v>
-      </c>
-      <c r="V33">
-        <v>43</v>
-      </c>
-      <c r="W33">
-        <v>12</v>
-      </c>
-      <c r="X33">
-        <v>1.2</v>
-      </c>
-      <c r="Y33">
-        <v>0.49</v>
-      </c>
-      <c r="Z33">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="AA33">
-        <v>0.47199999999999998</v>
-      </c>
-      <c r="AB33">
-        <v>7.5</v>
-      </c>
-      <c r="AC33">
-        <v>1</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34">
-        <v>367</v>
+        <v>26</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="D34">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E34">
-        <v>40</v>
+        <v>2.8</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>426</v>
+      </c>
+      <c r="H34">
+        <v>0.05</v>
+      </c>
+      <c r="I34">
+        <v>0.11</v>
+      </c>
+      <c r="J34">
+        <v>0.6</v>
+      </c>
+      <c r="K34">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="L34">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N34">
+        <v>16</v>
+      </c>
+      <c r="P34">
+        <v>9</v>
+      </c>
+      <c r="R34">
+        <v>1.06</v>
+      </c>
+      <c r="S34">
+        <v>1.1000000000000001</v>
       </c>
       <c r="T34">
-        <v>106</v>
+        <v>340</v>
       </c>
       <c r="U34">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="V34">
+        <v>44</v>
+      </c>
+      <c r="W34">
+        <v>12</v>
       </c>
       <c r="X34">
-        <v>1.0900000000000001</v>
+        <v>0.8</v>
+      </c>
+      <c r="Y34">
+        <v>0.32</v>
+      </c>
+      <c r="Z34">
+        <v>0.127</v>
+      </c>
+      <c r="AA34">
+        <v>0.125</v>
+      </c>
+      <c r="AB34">
+        <v>0.3</v>
       </c>
       <c r="AC34">
-        <v>106</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B35">
-        <v>36</v>
+        <v>359</v>
       </c>
       <c r="C35">
-        <v>0.22</v>
+        <v>1.3</v>
       </c>
       <c r="D35">
-        <v>7.96</v>
+        <v>79.8</v>
       </c>
       <c r="E35">
-        <v>4.8600000000000003</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>0.64</v>
-      </c>
-      <c r="M35">
-        <v>3.7</v>
-      </c>
-      <c r="P35">
-        <v>59.6</v>
+        <v>6.94</v>
+      </c>
+      <c r="H35">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="I35">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J35">
+        <v>1.48</v>
+      </c>
+      <c r="K35">
+        <v>0.39</v>
+      </c>
+      <c r="L35">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="N35">
+        <v>97</v>
+      </c>
+      <c r="R35">
+        <v>0.04</v>
       </c>
       <c r="T35">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="U35">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="V35">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="W35">
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="X35">
-        <v>0.26</v>
+        <v>1.2</v>
       </c>
       <c r="Y35">
-        <v>0.11</v>
+        <v>0.49</v>
       </c>
       <c r="Z35">
-        <v>3.5000000000000003E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="AA35">
-        <v>0.36799999999999999</v>
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AB35">
+        <v>7.5</v>
       </c>
       <c r="AC35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="C36">
-        <v>0.32</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>99.7</v>
+        <v>77</v>
       </c>
       <c r="E36">
-        <v>99.7</v>
+        <v>40</v>
       </c>
       <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>1.9E-2</v>
+        <v>7</v>
       </c>
       <c r="T36">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="U36">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="X36">
-        <v>0.05</v>
-      </c>
-      <c r="Y36">
-        <v>0.01</v>
-      </c>
-      <c r="Z36">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="AB36">
-        <v>0.6</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="AC36">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>0.22</v>
+      </c>
+      <c r="D37">
+        <v>7.96</v>
+      </c>
+      <c r="E37">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="F37">
+        <v>0.64</v>
+      </c>
+      <c r="M37">
+        <v>3.7</v>
+      </c>
+      <c r="P37">
+        <v>59.6</v>
+      </c>
+      <c r="T37">
+        <v>161</v>
+      </c>
+      <c r="U37">
+        <v>17</v>
+      </c>
+      <c r="V37">
+        <v>23</v>
+      </c>
+      <c r="W37">
+        <v>12.5</v>
+      </c>
+      <c r="X37">
+        <v>0.26</v>
+      </c>
+      <c r="Y37">
+        <v>0.11</v>
+      </c>
+      <c r="Z37">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AA37">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AC37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>385</v>
+      </c>
+      <c r="C38">
+        <v>0.32</v>
+      </c>
+      <c r="D38">
+        <v>99.7</v>
+      </c>
+      <c r="E38">
+        <v>99.7</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <v>0.05</v>
+      </c>
+      <c r="Y38">
+        <v>0.01</v>
+      </c>
+      <c r="Z38">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB38">
+        <v>0.6</v>
+      </c>
+      <c r="AC38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>18</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <v>0.2</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>3.9</v>
       </c>
-      <c r="E37">
+      <c r="E39">
         <v>2.6</v>
       </c>
-      <c r="F37">
+      <c r="F39">
         <v>0.9</v>
       </c>
-      <c r="G37">
+      <c r="G39">
         <v>42</v>
       </c>
-      <c r="H37">
+      <c r="H39">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="I37">
+      <c r="I39">
         <v>1.9E-2</v>
       </c>
-      <c r="J37">
+      <c r="J39">
         <v>0.59399999999999997</v>
       </c>
-      <c r="K37">
+      <c r="K39">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="L37">
+      <c r="L39">
         <v>0.08</v>
       </c>
-      <c r="N37">
+      <c r="N39">
         <v>15</v>
       </c>
-      <c r="P37">
+      <c r="P39">
         <v>13.7</v>
       </c>
-      <c r="R37">
+      <c r="R39">
         <v>0.54</v>
       </c>
-      <c r="S37">
+      <c r="S39">
         <v>7.9</v>
       </c>
-      <c r="T37">
+      <c r="T39">
         <v>237</v>
       </c>
-      <c r="U37">
+      <c r="U39">
         <v>10</v>
       </c>
-      <c r="V37">
+      <c r="V39">
         <v>24</v>
       </c>
-      <c r="W37">
+      <c r="W39">
         <v>11</v>
       </c>
-      <c r="X37">
+      <c r="X39">
         <v>0.27</v>
       </c>
-      <c r="Y37">
+      <c r="Y39">
         <v>0.17</v>
       </c>
-      <c r="Z37">
+      <c r="Z39">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="AC37">
+      <c r="AC39">
         <v>5</v>
       </c>
     </row>
@@ -2534,7 +2685,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38:G1048576 H37 G1:G36">
+  <conditionalFormatting sqref="G40:G1048576 H39 G1:G38">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2546,7 +2697,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:H1048576 I37 H1:H36">
+  <conditionalFormatting sqref="H40:H1048576 I39 H1:H38">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2558,7 +2709,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38:I1048576 J37 I1:I36">
+  <conditionalFormatting sqref="I40:I1048576 J39 I1:I38">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2570,7 +2721,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38:J1048576 J1:J36">
+  <conditionalFormatting sqref="J40:J1048576 J1:J38">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>